<commit_message>
Dashboard, Data, and Calculation
</commit_message>
<xml_diff>
--- a/My_KPI_Dashboard.xlsx
+++ b/My_KPI_Dashboard.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\idgre\Videos\Programming\Visually Effective Excel Dashboard\KPI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1766C4A3-361D-4ADF-9833-9C544511B273}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{542D9583-E8EE-4312-9919-C88879EA1851}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{FE35E5F9-BE9E-4FF4-9B14-4133B907AECB}"/>
+    <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="8880" activeTab="1" xr2:uid="{FE35E5F9-BE9E-4FF4-9B14-4133B907AECB}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="5" r:id="rId1"/>
@@ -1218,22 +1218,22 @@
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>Aviatrr</c:v>
+                  <c:v>Strex</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Hackrr</c:v>
+                  <c:v>Amplefio</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Baden</c:v>
+                  <c:v>Atmos</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Five Labs</c:v>
+                  <c:v>Scrap</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Pes</c:v>
+                  <c:v>Misty Wash</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Fightrr</c:v>
+                  <c:v>Accord</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1245,22 +1245,22 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>8126</c:v>
+                  <c:v>8152</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>18700.5</c:v>
+                  <c:v>8250</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>35980</c:v>
+                  <c:v>10675</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>21579</c:v>
+                  <c:v>13307</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>45315.9</c:v>
+                  <c:v>30399.599999999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>11649</c:v>
+                  <c:v>17760</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1333,22 +1333,22 @@
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>Aviatrr</c:v>
+                  <c:v>Strex</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Hackrr</c:v>
+                  <c:v>Amplefio</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Baden</c:v>
+                  <c:v>Atmos</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Five Labs</c:v>
+                  <c:v>Scrap</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Pes</c:v>
+                  <c:v>Misty Wash</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Fightrr</c:v>
+                  <c:v>Accord</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1360,22 +1360,22 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>8642</c:v>
+                  <c:v>9698</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>19101.600000000002</c:v>
+                  <c:v>8899</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>36362</c:v>
+                  <c:v>11178</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>20478</c:v>
+                  <c:v>13448</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43003.8</c:v>
+                  <c:v>30237.199999999997</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>10593</c:v>
+                  <c:v>16854</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1419,7 +1419,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D956E4CB-9B4B-4C1E-B3E8-D218D7D40EE2}" type="CELLRANGE">
+                    <a:fld id="{2CB65D42-F10F-447E-B222-81C70A6A4D53}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1452,7 +1452,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{546624BA-D59F-46B3-A278-11A7BD23773C}" type="CELLRANGE">
+                    <a:fld id="{B785FC1B-0725-440A-9CD8-70514DA17BBC}" type="CELLRANGE">
                       <a:rPr lang="en-NG"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1486,7 +1486,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D45F5419-6264-4B20-BCB5-08864B4CFD46}" type="CELLRANGE">
+                    <a:fld id="{8630BC35-9122-460D-A662-B3DCD8155975}" type="CELLRANGE">
                       <a:rPr lang="en-NG"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1520,7 +1520,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{187A275F-79A3-4632-B639-934F53B1A169}" type="CELLRANGE">
+                    <a:fld id="{0CC22D5A-E251-4AE1-864F-8B05A83AF236}" type="CELLRANGE">
                       <a:rPr lang="en-NG"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1554,7 +1554,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8B34DE7C-C99A-4765-9818-855FAFC552D8}" type="CELLRANGE">
+                    <a:fld id="{FDCE99DB-116E-4CCF-AC76-8FF325B28F60}" type="CELLRANGE">
                       <a:rPr lang="en-NG"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1588,7 +1588,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3E9D224D-7449-4F41-AE41-3EB939B0EAFE}" type="CELLRANGE">
+                    <a:fld id="{E81C1233-2EF3-46B2-A735-FDAEB90C5A05}" type="CELLRANGE">
                       <a:rPr lang="en-NG"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1682,22 +1682,22 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>8642</c:v>
+                  <c:v>9698</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>19101.600000000002</c:v>
+                  <c:v>8899</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>36362</c:v>
+                  <c:v>11178</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>21579</c:v>
+                  <c:v>13448</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>45315.9</c:v>
+                  <c:v>30399.599999999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>11649</c:v>
+                  <c:v>17760</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1710,22 +1710,22 @@
                 <c15:dlblRangeCache>
                   <c:ptCount val="6"/>
                   <c:pt idx="0">
-                    <c:v>-6% | 8,126</c:v>
+                    <c:v>-16% | 8,152</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>-2% | 18,701</c:v>
+                    <c:v>-7% | 8,250</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>-1% | 35,980</c:v>
+                    <c:v>-4% | 10,675</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>5% | 21,579</c:v>
+                    <c:v>-1% | 13,307</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>5% | 45,316</c:v>
+                    <c:v>1% | 30,400</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>10% | 11,649</c:v>
+                    <c:v>5% | 17,760</c:v>
                   </c:pt>
                 </c15:dlblRangeCache>
               </c15:datalabelsRange>
@@ -2056,40 +2056,40 @@
                 <c:formatCode>_-* #,##0_-;\-* #,##0_-;_-* "-"??_-;_-@_-</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>16</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>27</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>27</c:v>
+                  <c:v>89</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>105</c:v>
+                  <c:v>179</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>218</c:v>
+                  <c:v>234</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>309</c:v>
+                  <c:v>341</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>488</c:v>
+                  <c:v>459</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>464</c:v>
+                  <c:v>536</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>429</c:v>
+                  <c:v>629</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>430</c:v>
+                  <c:v>656</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>432</c:v>
+                  <c:v>641</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>435</c:v>
+                  <c:v>550</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2236,40 +2236,40 @@
                 <c:formatCode>_-* #,##0_-;\-* #,##0_-;_-* "-"??_-;_-@_-</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>22</c:v>
+                  <c:v>71</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>52</c:v>
+                  <c:v>142</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>90</c:v>
+                  <c:v>247</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>150</c:v>
+                  <c:v>307</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>258</c:v>
+                  <c:v>395</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>350</c:v>
+                  <c:v>461</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>458</c:v>
+                  <c:v>564</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>453</c:v>
+                  <c:v>645</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>522</c:v>
+                  <c:v>688</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>566</c:v>
+                  <c:v>706</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>596</c:v>
+                  <c:v>664</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>591</c:v>
+                  <c:v>593</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2358,22 +2358,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>17</c:v>
+                  <c:v>82</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>50</c:v>
+                  <c:v>134</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>67</c:v>
+                  <c:v>187</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>80</c:v>
+                  <c:v>244</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>122</c:v>
+                  <c:v>338</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>192</c:v>
+                  <c:v>408</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0</c:v>
@@ -2385,13 +2385,13 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>#N/A</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>#N/A</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>#N/A</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2504,7 +2504,7 @@
                   <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>#N/A</c:v>
@@ -2513,7 +2513,7 @@
                   <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>#N/A</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3789,7 +3789,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropLines="3" dropStyle="combo" dx="26" fmlaLink="Calculation!$D$4" fmlaRange="Calculation!$C$14:$C$16" noThreeD="1" sel="2" val="0"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropLines="3" dropStyle="combo" dx="26" fmlaLink="Calculation!$D$4" fmlaRange="Calculation!$C$14:$C$16" noThreeD="1" sel="3" val="0"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3797,7 +3797,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp3.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="List" dx="26" fmlaLink="Calculation!$D$6" fmlaRange="Calculation!$D$14:$D$16" noThreeD="1" sel="2" val="0"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="List" dx="26" fmlaLink="Calculation!$D$6" fmlaRange="Calculation!$D$14:$D$16" noThreeD="1" sel="1" val="0"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp4.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3809,7 +3809,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp6.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="26" fmlaLink="Calculation!$D$8" horiz="1" max="20" min="1" page="5" val="13"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="26" fmlaLink="Calculation!$D$8" horiz="1" max="20" min="1" page="5" val="3"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp7.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4128,7 +4128,7 @@
               <a:cs typeface="Arial"/>
             </a:rPr>
             <a:pPr algn="l"/>
-            <a:t>-$4,121 </a:t>
+            <a:t>-$3,314 </a:t>
           </a:fld>
           <a:endParaRPr lang="en-NG" sz="900">
             <a:solidFill>
@@ -4169,8 +4169,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="4099560" y="144780"/>
-          <a:ext cx="1607820" cy="1028700"/>
+          <a:off x="4113711" y="144780"/>
+          <a:ext cx="1613263" cy="1022169"/>
           <a:chOff x="4320540" y="144780"/>
           <a:chExt cx="1607820" cy="1028700"/>
         </a:xfrm>
@@ -4295,7 +4295,7 @@
                 <a:cs typeface="Arial"/>
               </a:rPr>
               <a:pPr algn="l"/>
-              <a:t> $12,090 </a:t>
+              <a:t> $8,514 </a:t>
             </a:fld>
             <a:endParaRPr lang="en-NG" sz="900">
               <a:solidFill>
@@ -4432,7 +4432,7 @@
                 <a:cs typeface="Arial"/>
               </a:rPr>
               <a:pPr algn="l"/>
-              <a:t> $210,616.00 </a:t>
+              <a:t> $189,978.50 </a:t>
             </a:fld>
             <a:endParaRPr lang="en-NG" sz="1400" b="0"/>
           </a:p>
@@ -4552,8 +4552,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="5692140" y="144780"/>
-          <a:ext cx="1706881" cy="998220"/>
+          <a:off x="5711734" y="144780"/>
+          <a:ext cx="1704704" cy="991689"/>
           <a:chOff x="5905500" y="144780"/>
           <a:chExt cx="1668781" cy="998220"/>
         </a:xfrm>
@@ -4678,7 +4678,7 @@
                 <a:cs typeface="Arial"/>
               </a:rPr>
               <a:pPr algn="l"/>
-              <a:t> $981 </a:t>
+              <a:t> $747 </a:t>
             </a:fld>
             <a:endParaRPr lang="en-NG" sz="900">
               <a:solidFill>
@@ -4815,7 +4815,7 @@
                 <a:cs typeface="Arial"/>
               </a:rPr>
               <a:pPr algn="l"/>
-              <a:t> $12,324.30 </a:t>
+              <a:t> $8,869.20 </a:t>
             </a:fld>
             <a:endParaRPr lang="en-NG" sz="1800" b="0"/>
           </a:p>
@@ -4891,7 +4891,7 @@
               <a:cs typeface="Arial"/>
             </a:rPr>
             <a:pPr algn="l"/>
-            <a:t>Game Apps</a:t>
+            <a:t>Utility Apps</a:t>
           </a:fld>
           <a:endParaRPr lang="en-NG" sz="2400" b="1"/>
         </a:p>
@@ -4966,7 +4966,7 @@
               <a:cs typeface="Arial"/>
             </a:rPr>
             <a:pPr algn="l"/>
-            <a:t> $95,902.10 </a:t>
+            <a:t> $91,467.10 </a:t>
           </a:fld>
           <a:endParaRPr lang="en-NG" sz="2400" b="0">
             <a:solidFill>
@@ -5496,7 +5496,7 @@
               <a:cs typeface="Arial"/>
             </a:rPr>
             <a:pPr algn="l"/>
-            <a:t>Profit for Arcade</a:t>
+            <a:t>Profit for Infic</a:t>
           </a:fld>
           <a:endParaRPr lang="en-NG" sz="1200" b="1">
             <a:solidFill>
@@ -5756,8 +5756,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="7406640" y="144780"/>
-          <a:ext cx="2019300" cy="1013460"/>
+          <a:off x="7424057" y="144780"/>
+          <a:ext cx="2034540" cy="1006929"/>
           <a:chOff x="7368540" y="144780"/>
           <a:chExt cx="2019300" cy="1013460"/>
         </a:xfrm>
@@ -5882,7 +5882,7 @@
                 <a:cs typeface="Arial"/>
               </a:rPr>
               <a:pPr algn="l"/>
-              <a:t>-$4,121 </a:t>
+              <a:t>-$3,314 </a:t>
             </a:fld>
             <a:endParaRPr lang="en-NG" sz="900">
               <a:solidFill>
@@ -6019,7 +6019,7 @@
                 <a:cs typeface="Arial"/>
               </a:rPr>
               <a:pPr algn="l"/>
-              <a:t> $95,902.10 </a:t>
+              <a:t> $91,467.10 </a:t>
             </a:fld>
             <a:endParaRPr lang="en-NG" sz="2400" b="0">
               <a:solidFill>
@@ -7315,7 +7315,7 @@
   <dimension ref="A1:AT51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+      <selection activeCell="C38" sqref="A1:C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -7401,39 +7401,39 @@
     <row r="4" spans="1:46" x14ac:dyDescent="0.25">
       <c r="B4" t="str">
         <f t="shared" ref="B4:AT4" si="0">B5&amp;B6&amp;B7&amp;B8</f>
-        <v>2024SepActualRevenue</v>
+        <v>2024DecActualRevenue</v>
       </c>
       <c r="C4" t="str">
         <f t="shared" si="0"/>
-        <v>2024SepActualProfit</v>
+        <v>2024DecActualProfit</v>
       </c>
       <c r="D4" s="12" t="str">
         <f t="shared" si="0"/>
-        <v>2024SepActualCash</v>
+        <v>2024DecActualCash</v>
       </c>
       <c r="E4" t="str">
         <f t="shared" si="0"/>
-        <v>2023SepActualRevenue</v>
+        <v>2023DecActualRevenue</v>
       </c>
       <c r="F4" t="str">
         <f t="shared" si="0"/>
-        <v>2023SepActualProfit</v>
+        <v>2023DecActualProfit</v>
       </c>
       <c r="G4" s="12" t="str">
         <f t="shared" si="0"/>
-        <v>2023SepActualCash</v>
+        <v>2023DecActualCash</v>
       </c>
       <c r="H4" t="str">
         <f t="shared" si="0"/>
-        <v>2024SepBudgetRevenue</v>
+        <v>2024DecBudgetRevenue</v>
       </c>
       <c r="I4" t="str">
         <f t="shared" si="0"/>
-        <v>2024SepBudgetProfit</v>
+        <v>2024DecBudgetProfit</v>
       </c>
       <c r="J4" s="12" t="str">
         <f t="shared" si="0"/>
-        <v>2024SepBudgetCash</v>
+        <v>2024DecBudgetCash</v>
       </c>
       <c r="K4" s="13" t="str">
         <f t="shared" si="0"/>
@@ -7765,39 +7765,39 @@
     <row r="6" spans="1:46" x14ac:dyDescent="0.25">
       <c r="B6" s="16" t="str">
         <f t="shared" ref="B6:J6" si="7">cur_month</f>
-        <v>Sep</v>
+        <v>Dec</v>
       </c>
       <c r="C6" s="16" t="str">
         <f t="shared" si="7"/>
-        <v>Sep</v>
+        <v>Dec</v>
       </c>
       <c r="D6" s="17" t="str">
         <f t="shared" si="7"/>
-        <v>Sep</v>
+        <v>Dec</v>
       </c>
       <c r="E6" s="16" t="str">
         <f t="shared" si="7"/>
-        <v>Sep</v>
+        <v>Dec</v>
       </c>
       <c r="F6" s="16" t="str">
         <f t="shared" si="7"/>
-        <v>Sep</v>
+        <v>Dec</v>
       </c>
       <c r="G6" s="17" t="str">
         <f t="shared" si="7"/>
-        <v>Sep</v>
+        <v>Dec</v>
       </c>
       <c r="H6" s="16" t="str">
         <f t="shared" si="7"/>
-        <v>Sep</v>
+        <v>Dec</v>
       </c>
       <c r="I6" s="16" t="str">
         <f t="shared" si="7"/>
-        <v>Sep</v>
+        <v>Dec</v>
       </c>
       <c r="J6" s="17" t="str">
         <f t="shared" si="7"/>
-        <v>Sep</v>
+        <v>Dec</v>
       </c>
       <c r="K6" s="18" t="s">
         <v>18</v>
@@ -13610,7 +13610,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="RBGDjFmgniOqhglp4g7UxQvuK6lqyfvaQ5N9iazA7yWOcCe8IdPqui3pPKuCnMOu0grAkKfOi0T0o7Sc1W5Ijg==" saltValue="A7g5pZoF6TsvxvgqvCafcg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -13623,8 +13622,8 @@
   </sheetPr>
   <dimension ref="A1:AE45"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="T16" sqref="T16"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="13.8" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -13770,7 +13769,7 @@
         <v>76</v>
       </c>
       <c r="F5" s="95" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="G5" s="59"/>
       <c r="H5" s="33"/>
@@ -13964,23 +13963,23 @@
       </c>
       <c r="E11" t="str" cm="1">
         <f t="array" ref="E11">INDEX(Calculation!N14:N$34,Calculation!$D$5)</f>
-        <v>Fightrr</v>
+        <v>Commuta</v>
       </c>
       <c r="F11" s="56" cm="1">
         <f t="array" ref="F11">INDEX(Calculation!O14:O$34,Calculation!$D$5)</f>
-        <v>11649</v>
+        <v>6353</v>
       </c>
       <c r="H11" s="54" cm="1">
         <f t="array" ref="H11">INDEX(Calculation!X14:X$34,Calculation!$D$5)</f>
-        <v>0.11859035913193777</v>
+        <v>6.0070081762055728E-2</v>
       </c>
       <c r="I11" s="57">
         <f>H11</f>
-        <v>0.11859035913193777</v>
+        <v>6.0070081762055728E-2</v>
       </c>
       <c r="K11" s="54" cm="1">
         <f t="array" ref="K11">INDEX(Calculation!AA14:AA$34,Calculation!$D$5)</f>
-        <v>9.9688473520249218E-2</v>
+        <v>0.20436018957345972</v>
       </c>
       <c r="L11" s="81" t="str">
         <f>IF(K11="","",IF(K11&lt;-0.05,"▼",IF(K11&gt;0.05,"▲","")))</f>
@@ -13988,19 +13987,19 @@
       </c>
       <c r="M11" s="56" cm="1">
         <f t="array" ref="M11">INDEX(Calculation!P14:P$34,Calculation!$D$5)</f>
-        <v>802</v>
+        <v>762</v>
       </c>
       <c r="O11" s="54" cm="1">
         <f t="array" ref="O11">INDEX(Calculation!Y14:Y$34,Calculation!$D$5)</f>
-        <v>0.4962686567164179</v>
+        <v>0.13056379821958458</v>
       </c>
       <c r="P11" s="57">
         <f>O11</f>
-        <v>0.4962686567164179</v>
+        <v>0.13056379821958458</v>
       </c>
       <c r="R11" s="54" cm="1">
         <f t="array" ref="R11">INDEX(Calculation!AB14:AB$34,Calculation!$D$5)</f>
-        <v>0.44765342960288806</v>
+        <v>0.34154929577464788</v>
       </c>
       <c r="S11" s="81" t="str">
         <f>IF(R11="","",IF(R11&lt;-0.05,"▼",IF(R11&gt;0.05,"▲","")))</f>
@@ -14008,23 +14007,23 @@
       </c>
       <c r="T11" s="56" cm="1">
         <f t="array" ref="T11">INDEX(Calculation!Q14:Q$34,Calculation!$D$5)</f>
-        <v>5956</v>
+        <v>7332</v>
       </c>
       <c r="V11" s="54" cm="1">
         <f t="array" ref="V11">INDEX(Calculation!Z14:Z$34,Calculation!$D$5)</f>
-        <v>-0.11276627439296887</v>
+        <v>2.3022185014650483E-2</v>
       </c>
       <c r="W11" s="57">
         <f>V11</f>
-        <v>-0.11276627439296887</v>
+        <v>2.3022185014650483E-2</v>
       </c>
       <c r="Y11" s="54" cm="1">
         <f t="array" ref="Y11">INDEX(Calculation!AC14:AC$34,Calculation!$D$5)</f>
-        <v>-0.12450389534029105</v>
+        <v>1.4528850145288501E-2</v>
       </c>
       <c r="Z11" s="37" t="str">
         <f>IF(Y11="","",IF(Y11&lt;-0.05,"▼",IF(Y11&gt;0.05,"▲","")))</f>
-        <v>▼</v>
+        <v/>
       </c>
       <c r="AB11" s="33"/>
       <c r="AC11" s="33"/>
@@ -14040,25 +14039,25 @@
       </c>
       <c r="E12" s="60" t="str" cm="1">
         <f t="array" ref="E12">INDEX(Calculation!N15:N$34,Calculation!$D$5)</f>
-        <v>Kryptis</v>
+        <v>Infic</v>
       </c>
       <c r="F12" s="61" cm="1">
         <f t="array" ref="F12">INDEX(Calculation!O15:O$34,Calculation!$D$5)</f>
-        <v>7718</v>
+        <v>12373</v>
       </c>
       <c r="G12" s="60"/>
       <c r="H12" s="62" cm="1">
         <f t="array" ref="H12">INDEX(Calculation!X15:X$34,Calculation!$D$5)</f>
-        <v>5.9873661082120298E-2</v>
+        <v>-2.0164542668172285E-3</v>
       </c>
       <c r="I12" s="63">
         <f t="shared" ref="I12:I20" si="0">H12</f>
-        <v>5.9873661082120298E-2</v>
+        <v>-2.0164542668172285E-3</v>
       </c>
       <c r="J12" s="60"/>
       <c r="K12" s="62" cm="1">
         <f t="array" ref="K12">INDEX(Calculation!AA15:AA$34,Calculation!$D$5)</f>
-        <v>0.20424403183023873</v>
+        <v>0.18153170359052712</v>
       </c>
       <c r="L12" s="82" t="str">
         <f t="shared" ref="L12:L20" si="1">IF(K12="","",IF(K12&lt;-0.05,"▼",IF(K12&gt;0.05,"▲","")))</f>
@@ -14066,43 +14065,43 @@
       </c>
       <c r="M12" s="61" cm="1">
         <f t="array" ref="M12">INDEX(Calculation!P15:P$34,Calculation!$D$5)</f>
-        <v>876</v>
+        <v>408</v>
       </c>
       <c r="N12" s="60"/>
       <c r="O12" s="62" cm="1">
         <f t="array" ref="O12">INDEX(Calculation!Y15:Y$34,Calculation!$D$5)</f>
-        <v>0.13032258064516128</v>
+        <v>0.19648093841642228</v>
       </c>
       <c r="P12" s="63">
         <f t="shared" ref="P12:P20" si="2">O12</f>
-        <v>0.13032258064516128</v>
+        <v>0.19648093841642228</v>
       </c>
       <c r="Q12" s="60"/>
       <c r="R12" s="62" cm="1">
         <f t="array" ref="R12">INDEX(Calculation!AB15:AB$34,Calculation!$D$5)</f>
-        <v>0.33944954128440369</v>
+        <v>-0.11496746203904555</v>
       </c>
       <c r="S12" s="82" t="str">
         <f t="shared" ref="S12:S20" si="3">IF(R12="","",IF(R12&lt;-0.05,"▼",IF(R12&gt;0.05,"▲","")))</f>
-        <v>▲</v>
+        <v>▼</v>
       </c>
       <c r="T12" s="61" cm="1">
         <f t="array" ref="T12">INDEX(Calculation!Q15:Q$34,Calculation!$D$5)</f>
-        <v>8432</v>
+        <v>3054</v>
       </c>
       <c r="U12" s="60"/>
       <c r="V12" s="62" cm="1">
         <f t="array" ref="V12">INDEX(Calculation!Z15:Z$34,Calculation!$D$5)</f>
-        <v>2.3052657122057753E-2</v>
+        <v>6.923837784371909E-3</v>
       </c>
       <c r="W12" s="63">
         <f t="shared" ref="W12:W20" si="4">V12</f>
-        <v>2.3052657122057753E-2</v>
+        <v>6.923837784371909E-3</v>
       </c>
       <c r="X12" s="60"/>
       <c r="Y12" s="62" cm="1">
         <f t="array" ref="Y12">INDEX(Calculation!AC15:AC$34,Calculation!$D$5)</f>
-        <v>1.4436958614051972E-2</v>
+        <v>4.9484536082474224E-2</v>
       </c>
       <c r="Z12" s="64" t="str">
         <f t="shared" ref="Z12:Z20" si="5">IF(Y12="","",IF(Y12&lt;-0.05,"▼",IF(Y12&gt;0.05,"▲","")))</f>
@@ -14122,23 +14121,23 @@
       </c>
       <c r="E13" t="str" cm="1">
         <f t="array" ref="E13">INDEX(Calculation!N16:N$34,Calculation!$D$5)</f>
-        <v>Perino</v>
+        <v>Accord</v>
       </c>
       <c r="F13" s="56" cm="1">
         <f t="array" ref="F13">INDEX(Calculation!O16:O$34,Calculation!$D$5)</f>
-        <v>15033</v>
+        <v>17760</v>
       </c>
       <c r="H13" s="54" cm="1">
         <f t="array" ref="H13">INDEX(Calculation!X16:X$34,Calculation!$D$5)</f>
-        <v>-2.0578863515666491E-3</v>
+        <v>4.3171806167400878E-2</v>
       </c>
       <c r="I13" s="57">
         <f t="shared" si="0"/>
-        <v>-2.0578863515666491E-3</v>
+        <v>4.3171806167400878E-2</v>
       </c>
       <c r="K13" s="54" cm="1">
         <f t="array" ref="K13">INDEX(Calculation!AA16:AA$34,Calculation!$D$5)</f>
-        <v>0.18146809179503301</v>
+        <v>5.3755784976860094E-2</v>
       </c>
       <c r="L13" s="81" t="str">
         <f t="shared" si="1"/>
@@ -14146,39 +14145,39 @@
       </c>
       <c r="M13" s="56" cm="1">
         <f t="array" ref="M13">INDEX(Calculation!P16:P$34,Calculation!$D$5)</f>
-        <v>469</v>
+        <v>800</v>
       </c>
       <c r="O13" s="54" cm="1">
         <f t="array" ref="O13">INDEX(Calculation!Y16:Y$34,Calculation!$D$5)</f>
-        <v>0.19642857142857142</v>
+        <v>0.40845070422535212</v>
       </c>
       <c r="P13" s="57">
         <f t="shared" si="2"/>
-        <v>0.19642857142857142</v>
+        <v>0.40845070422535212</v>
       </c>
       <c r="R13" s="54" cm="1">
         <f t="array" ref="R13">INDEX(Calculation!AB16:AB$34,Calculation!$D$5)</f>
-        <v>-0.11509433962264151</v>
+        <v>0.39860139860139859</v>
       </c>
       <c r="S13" s="81" t="str">
         <f t="shared" si="3"/>
-        <v>▼</v>
+        <v>▲</v>
       </c>
       <c r="T13" s="56" cm="1">
         <f t="array" ref="T13">INDEX(Calculation!Q16:Q$34,Calculation!$D$5)</f>
-        <v>3512</v>
+        <v>6488</v>
       </c>
       <c r="V13" s="54" cm="1">
         <f t="array" ref="V13">INDEX(Calculation!Z16:Z$34,Calculation!$D$5)</f>
-        <v>6.8807339449541288E-3</v>
+        <v>-0.13134288392020352</v>
       </c>
       <c r="W13" s="57">
         <f t="shared" si="4"/>
-        <v>6.8807339449541288E-3</v>
+        <v>-0.13134288392020352</v>
       </c>
       <c r="Y13" s="54" cm="1">
         <f t="array" ref="Y13">INDEX(Calculation!AC16:AC$34,Calculation!$D$5)</f>
-        <v>4.9297878697340904E-2</v>
+        <v>-1.8605354711843897E-2</v>
       </c>
       <c r="Z13" s="37" t="str">
         <f t="shared" si="5"/>
@@ -14198,73 +14197,73 @@
       </c>
       <c r="E14" s="60" t="str" cm="1">
         <f t="array" ref="E14">INDEX(Calculation!N17:N$34,Calculation!$D$5)</f>
-        <v>Five Labs</v>
+        <v>Misty Wash</v>
       </c>
       <c r="F14" s="61" cm="1">
         <f t="array" ref="F14">INDEX(Calculation!O17:O$34,Calculation!$D$5)</f>
-        <v>21579</v>
+        <v>30399.599999999999</v>
       </c>
       <c r="G14" s="60"/>
       <c r="H14" s="62" cm="1">
         <f t="array" ref="H14">INDEX(Calculation!X17:X$34,Calculation!$D$5)</f>
-        <v>4.3169293241806052E-2</v>
+        <v>2.9392244240068269E-2</v>
       </c>
       <c r="I14" s="63">
         <f t="shared" si="0"/>
-        <v>4.3169293241806052E-2</v>
+        <v>2.9392244240068269E-2</v>
       </c>
       <c r="J14" s="60"/>
       <c r="K14" s="62" cm="1">
         <f t="array" ref="K14">INDEX(Calculation!AA17:AA$34,Calculation!$D$5)</f>
-        <v>5.3765016114854965E-2</v>
+        <v>5.3708676729327274E-3</v>
       </c>
       <c r="L14" s="82" t="str">
         <f t="shared" si="1"/>
-        <v>▲</v>
+        <v/>
       </c>
       <c r="M14" s="61" cm="1">
         <f t="array" ref="M14">INDEX(Calculation!P17:P$34,Calculation!$D$5)</f>
-        <v>920</v>
+        <v>786.8</v>
       </c>
       <c r="N14" s="60"/>
       <c r="O14" s="62" cm="1">
         <f t="array" ref="O14">INDEX(Calculation!Y17:Y$34,Calculation!$D$5)</f>
-        <v>0.40888208269525267</v>
+        <v>0</v>
       </c>
       <c r="P14" s="63">
         <f t="shared" si="2"/>
-        <v>0.40888208269525267</v>
+        <v>0</v>
       </c>
       <c r="Q14" s="60"/>
       <c r="R14" s="62" cm="1">
         <f t="array" ref="R14">INDEX(Calculation!AB17:AB$34,Calculation!$D$5)</f>
-        <v>0.3981762917933131</v>
+        <v>-0.15615615615615619</v>
       </c>
       <c r="S14" s="82" t="str">
         <f t="shared" si="3"/>
-        <v>▲</v>
+        <v>▼</v>
       </c>
       <c r="T14" s="61" cm="1">
         <f t="array" ref="T14">INDEX(Calculation!Q17:Q$34,Calculation!$D$5)</f>
-        <v>7461</v>
+        <v>12308.8</v>
       </c>
       <c r="U14" s="60"/>
       <c r="V14" s="62" cm="1">
         <f t="array" ref="V14">INDEX(Calculation!Z17:Z$34,Calculation!$D$5)</f>
-        <v>-0.13133077191756898</v>
+        <v>-0.11709178549909618</v>
       </c>
       <c r="W14" s="63">
         <f t="shared" si="4"/>
-        <v>-0.13133077191756898</v>
+        <v>-0.11709178549909618</v>
       </c>
       <c r="X14" s="60"/>
       <c r="Y14" s="62" cm="1">
         <f t="array" ref="Y14">INDEX(Calculation!AC17:AC$34,Calculation!$D$5)</f>
-        <v>-1.8547750591949488E-2</v>
+        <v>-8.014228918183719E-2</v>
       </c>
       <c r="Z14" s="64" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>▼</v>
       </c>
       <c r="AA14" s="60"/>
       <c r="AB14" s="33"/>
@@ -14280,23 +14279,23 @@
       </c>
       <c r="E15" t="str" cm="1">
         <f t="array" ref="E15">INDEX(Calculation!N18:N$34,Calculation!$D$5)</f>
-        <v>Twistrr</v>
+        <v>Twenty20</v>
       </c>
       <c r="F15" s="56" cm="1">
         <f t="array" ref="F15">INDEX(Calculation!O18:O$34,Calculation!$D$5)</f>
-        <v>27210.600000000002</v>
+        <v>20400</v>
       </c>
       <c r="H15" s="54" cm="1">
         <f t="array" ref="H15">INDEX(Calculation!X18:X$34,Calculation!$D$5)</f>
-        <v>6.9246003678030868E-2</v>
+        <v>-8.2073434125269976E-2</v>
       </c>
       <c r="I15" s="57">
         <f t="shared" si="0"/>
-        <v>6.9246003678030868E-2</v>
+        <v>-8.2073434125269976E-2</v>
       </c>
       <c r="K15" s="54" cm="1">
         <f t="array" ref="K15">INDEX(Calculation!AA18:AA$34,Calculation!$D$5)</f>
-        <v>0.12352285395763665</v>
+        <v>0.10408728784205061</v>
       </c>
       <c r="L15" s="81" t="str">
         <f t="shared" si="1"/>
@@ -14304,43 +14303,43 @@
       </c>
       <c r="M15" s="56" cm="1">
         <f t="array" ref="M15">INDEX(Calculation!P18:P$34,Calculation!$D$5)</f>
-        <v>2903.4</v>
+        <v>614.40000000000009</v>
       </c>
       <c r="O15" s="54" cm="1">
         <f t="array" ref="O15">INDEX(Calculation!Y18:Y$34,Calculation!$D$5)</f>
-        <v>0.34416666666666673</v>
+        <v>-0.37864077669902907</v>
       </c>
       <c r="P15" s="57">
         <f t="shared" si="2"/>
-        <v>0.34416666666666673</v>
+        <v>-0.37864077669902907</v>
       </c>
       <c r="R15" s="54" cm="1">
         <f t="array" ref="R15">INDEX(Calculation!AB18:AB$34,Calculation!$D$5)</f>
-        <v>0.15214285714285719</v>
+        <v>-0.45142857142857135</v>
       </c>
       <c r="S15" s="81" t="str">
         <f t="shared" si="3"/>
-        <v>▲</v>
+        <v>▼</v>
       </c>
       <c r="T15" s="56" cm="1">
         <f t="array" ref="T15">INDEX(Calculation!Q18:Q$34,Calculation!$D$5)</f>
-        <v>10490.4</v>
+        <v>15171.2</v>
       </c>
       <c r="V15" s="54" cm="1">
         <f t="array" ref="V15">INDEX(Calculation!Z18:Z$34,Calculation!$D$5)</f>
-        <v>-6.1815840309079266E-2</v>
+        <v>-5.2936476228525764E-2</v>
       </c>
       <c r="W15" s="57">
         <f t="shared" si="4"/>
-        <v>-6.1815840309079266E-2</v>
+        <v>-5.2936476228525764E-2</v>
       </c>
       <c r="Y15" s="54" cm="1">
         <f t="array" ref="Y15">INDEX(Calculation!AC18:AC$34,Calculation!$D$5)</f>
-        <v>3.0981067125645089E-3</v>
+        <v>6.6111985608275178E-2</v>
       </c>
       <c r="Z15" s="37" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>▲</v>
       </c>
       <c r="AB15" s="33"/>
       <c r="AC15" s="33"/>
@@ -14356,73 +14355,73 @@
       </c>
       <c r="E16" s="60" t="str" cm="1">
         <f t="array" ref="E16">INDEX(Calculation!N19:N$34,Calculation!$D$5)</f>
-        <v>Hackrr</v>
+        <v>Tanox</v>
       </c>
       <c r="F16" s="61" cm="1">
         <f t="array" ref="F16">INDEX(Calculation!O19:O$34,Calculation!$D$5)</f>
-        <v>18700.5</v>
+        <v>21088</v>
       </c>
       <c r="G16" s="60"/>
       <c r="H16" s="62" cm="1">
         <f t="array" ref="H16">INDEX(Calculation!X19:X$34,Calculation!$D$5)</f>
-        <v>1.2391996361982599E-2</v>
+        <v>6.8504256181597084E-2</v>
       </c>
       <c r="I16" s="63">
         <f t="shared" si="0"/>
-        <v>1.2391996361982599E-2</v>
+        <v>6.8504256181597084E-2</v>
       </c>
       <c r="J16" s="60"/>
       <c r="K16" s="62" cm="1">
         <f t="array" ref="K16">INDEX(Calculation!AA19:AA$34,Calculation!$D$5)</f>
-        <v>-2.0998240985048485E-2</v>
+        <v>0.10085612862810607</v>
       </c>
       <c r="L16" s="82" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>▲</v>
       </c>
       <c r="M16" s="61" cm="1">
         <f t="array" ref="M16">INDEX(Calculation!P19:P$34,Calculation!$D$5)</f>
-        <v>984.90000000000009</v>
+        <v>1264</v>
       </c>
       <c r="N16" s="60"/>
       <c r="O16" s="62" cm="1">
         <f t="array" ref="O16">INDEX(Calculation!Y19:Y$34,Calculation!$D$5)</f>
-        <v>0.4841772151898735</v>
+        <v>0.35622317596566522</v>
       </c>
       <c r="P16" s="63">
         <f t="shared" si="2"/>
-        <v>0.4841772151898735</v>
+        <v>0.35622317596566522</v>
       </c>
       <c r="Q16" s="60"/>
       <c r="R16" s="62" cm="1">
         <f t="array" ref="R16">INDEX(Calculation!AB19:AB$34,Calculation!$D$5)</f>
-        <v>-0.24354838709677412</v>
+        <v>0.4697674418604651</v>
       </c>
       <c r="S16" s="82" t="str">
         <f t="shared" si="3"/>
-        <v>▼</v>
+        <v>▲</v>
       </c>
       <c r="T16" s="61" cm="1">
         <f t="array" ref="T16">INDEX(Calculation!Q19:Q$34,Calculation!$D$5)</f>
-        <v>12654.6</v>
+        <v>4828</v>
       </c>
       <c r="U16" s="60"/>
       <c r="V16" s="62" cm="1">
         <f t="array" ref="V16">INDEX(Calculation!Z19:Z$34,Calculation!$D$5)</f>
-        <v>-3.5994240921452564E-2</v>
+        <v>-0.18720538720538721</v>
       </c>
       <c r="W16" s="63">
         <f t="shared" si="4"/>
-        <v>-3.5994240921452564E-2</v>
+        <v>-0.18720538720538721</v>
       </c>
       <c r="X16" s="60"/>
       <c r="Y16" s="62" cm="1">
         <f t="array" ref="Y16">INDEX(Calculation!AC19:AC$34,Calculation!$D$5)</f>
-        <v>3.8249483115093103E-2</v>
+        <v>-0.37654958677685951</v>
       </c>
       <c r="Z16" s="64" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>▼</v>
       </c>
       <c r="AA16" s="60"/>
       <c r="AB16" s="33"/>
@@ -14438,23 +14437,23 @@
       </c>
       <c r="E17" t="str" cm="1">
         <f t="array" ref="E17">INDEX(Calculation!N20:N$34,Calculation!$D$5)</f>
-        <v>Pes</v>
+        <v>Minor Liar</v>
       </c>
       <c r="F17" s="56" cm="1">
         <f t="array" ref="F17">INDEX(Calculation!O20:O$34,Calculation!$D$5)</f>
-        <v>45315.9</v>
+        <v>23736.9</v>
       </c>
       <c r="H17" s="54" cm="1">
         <f t="array" ref="H17">INDEX(Calculation!X20:X$34,Calculation!$D$5)</f>
-        <v>4.3169293241806121E-2</v>
+        <v>4.3169293241806017E-2</v>
       </c>
       <c r="I17" s="57">
         <f t="shared" si="0"/>
-        <v>4.3169293241806121E-2</v>
+        <v>4.3169293241806017E-2</v>
       </c>
       <c r="K17" s="54" cm="1">
         <f t="array" ref="K17">INDEX(Calculation!AA20:AA$34,Calculation!$D$5)</f>
-        <v>5.376501611485493E-2</v>
+        <v>5.3765016114854895E-2</v>
       </c>
       <c r="L17" s="81" t="str">
         <f t="shared" si="1"/>
@@ -14462,7 +14461,7 @@
       </c>
       <c r="M17" s="56" cm="1">
         <f t="array" ref="M17">INDEX(Calculation!P20:P$34,Calculation!$D$5)</f>
-        <v>1932</v>
+        <v>1012.0000000000001</v>
       </c>
       <c r="O17" s="54" cm="1">
         <f t="array" ref="O17">INDEX(Calculation!Y20:Y$34,Calculation!$D$5)</f>
@@ -14482,19 +14481,19 @@
       </c>
       <c r="T17" s="56" cm="1">
         <f t="array" ref="T17">INDEX(Calculation!Q20:Q$34,Calculation!$D$5)</f>
-        <v>15668.1</v>
+        <v>8207.1</v>
       </c>
       <c r="V17" s="54" cm="1">
         <f t="array" ref="V17">INDEX(Calculation!Z20:Z$34,Calculation!$D$5)</f>
-        <v>-0.13133077191756903</v>
+        <v>-0.13133077191756909</v>
       </c>
       <c r="W17" s="57">
         <f t="shared" si="4"/>
-        <v>-0.13133077191756903</v>
+        <v>-0.13133077191756909</v>
       </c>
       <c r="Y17" s="54" cm="1">
         <f t="array" ref="Y17">INDEX(Calculation!AC20:AC$34,Calculation!$D$5)</f>
-        <v>-1.8547750591949509E-2</v>
+        <v>-1.8547750591949529E-2</v>
       </c>
       <c r="Z17" s="37" t="str">
         <f t="shared" si="5"/>
@@ -14514,73 +14513,73 @@
       </c>
       <c r="E18" s="60" t="str" cm="1">
         <f t="array" ref="E18">INDEX(Calculation!N21:N$34,Calculation!$D$5)</f>
-        <v>Baden</v>
+        <v>Mosquit</v>
       </c>
       <c r="F18" s="61" cm="1">
         <f t="array" ref="F18">INDEX(Calculation!O21:O$34,Calculation!$D$5)</f>
-        <v>35980</v>
+        <v>6302</v>
       </c>
       <c r="G18" s="60"/>
       <c r="H18" s="62" cm="1">
         <f t="array" ref="H18">INDEX(Calculation!X21:X$34,Calculation!$D$5)</f>
-        <v>9.728575785300396E-2</v>
+        <v>0.16703703703703704</v>
       </c>
       <c r="I18" s="63">
         <f t="shared" si="0"/>
-        <v>9.728575785300396E-2</v>
+        <v>0.16703703703703704</v>
       </c>
       <c r="J18" s="60"/>
       <c r="K18" s="62" cm="1">
         <f t="array" ref="K18">INDEX(Calculation!AA21:AA$34,Calculation!$D$5)</f>
-        <v>-1.0505472746273583E-2</v>
+        <v>0.19062913281692803</v>
       </c>
       <c r="L18" s="82" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>▲</v>
       </c>
       <c r="M18" s="61" cm="1">
         <f t="array" ref="M18">INDEX(Calculation!P21:P$34,Calculation!$D$5)</f>
-        <v>2332</v>
+        <v>240</v>
       </c>
       <c r="N18" s="60"/>
       <c r="O18" s="62" cm="1">
         <f t="array" ref="O18">INDEX(Calculation!Y21:Y$34,Calculation!$D$5)</f>
-        <v>0.16251246261216351</v>
+        <v>0.26315789473684209</v>
       </c>
       <c r="P18" s="63">
         <f t="shared" si="2"/>
-        <v>0.16251246261216351</v>
+        <v>0.26315789473684209</v>
       </c>
       <c r="Q18" s="60"/>
       <c r="R18" s="62" cm="1">
         <f t="array" ref="R18">INDEX(Calculation!AB21:AB$34,Calculation!$D$5)</f>
-        <v>-4.6606704824202781E-2</v>
+        <v>0.53846153846153844</v>
       </c>
       <c r="S18" s="82" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>▲</v>
       </c>
       <c r="T18" s="61" cm="1">
         <f t="array" ref="T18">INDEX(Calculation!Q21:Q$34,Calculation!$D$5)</f>
-        <v>14274</v>
+        <v>4655</v>
       </c>
       <c r="U18" s="60"/>
       <c r="V18" s="62" cm="1">
         <f t="array" ref="V18">INDEX(Calculation!Z21:Z$34,Calculation!$D$5)</f>
-        <v>-3.8528896672504379E-2</v>
+        <v>0.136474609375</v>
       </c>
       <c r="W18" s="63">
         <f t="shared" si="4"/>
-        <v>-3.8528896672504379E-2</v>
+        <v>0.136474609375</v>
       </c>
       <c r="X18" s="60"/>
       <c r="Y18" s="62" cm="1">
         <f t="array" ref="Y18">INDEX(Calculation!AC21:AC$34,Calculation!$D$5)</f>
-        <v>-0.12920937042459738</v>
+        <v>3.1236154186973859E-2</v>
       </c>
       <c r="Z18" s="64" t="str">
         <f t="shared" si="5"/>
-        <v>▼</v>
+        <v/>
       </c>
       <c r="AA18" s="60"/>
       <c r="AB18" s="33"/>
@@ -14596,63 +14595,63 @@
       </c>
       <c r="E19" t="str" cm="1">
         <f t="array" ref="E19">INDEX(Calculation!N22:N$34,Calculation!$D$5)</f>
-        <v>Jellyfish</v>
+        <v>Atmos</v>
       </c>
       <c r="F19" s="56" cm="1">
         <f t="array" ref="F19">INDEX(Calculation!O22:O$34,Calculation!$D$5)</f>
-        <v>7657</v>
+        <v>10675</v>
       </c>
       <c r="H19" s="54" cm="1">
         <f t="array" ref="H19">INDEX(Calculation!X22:X$34,Calculation!$D$5)</f>
-        <v>0.44281138119464858</v>
+        <v>5.34886015987368E-2</v>
       </c>
       <c r="I19" s="57">
         <f t="shared" si="0"/>
-        <v>0.44281138119464858</v>
+        <v>5.34886015987368E-2</v>
       </c>
       <c r="K19" s="54" cm="1">
         <f t="array" ref="K19">INDEX(Calculation!AA22:AA$34,Calculation!$D$5)</f>
-        <v>0.19063909189861608</v>
+        <v>-4.4999105385578816E-2</v>
       </c>
       <c r="L19" s="81" t="str">
         <f t="shared" si="1"/>
-        <v>▲</v>
+        <v/>
       </c>
       <c r="M19" s="56" cm="1">
         <f t="array" ref="M19">INDEX(Calculation!P22:P$34,Calculation!$D$5)</f>
-        <v>276</v>
+        <v>128</v>
       </c>
       <c r="O19" s="54" cm="1">
         <f t="array" ref="O19">INDEX(Calculation!Y22:Y$34,Calculation!$D$5)</f>
-        <v>0.62352941176470589</v>
+        <v>0.43820224719101125</v>
       </c>
       <c r="P19" s="57">
         <f t="shared" si="2"/>
-        <v>0.62352941176470589</v>
+        <v>0.43820224719101125</v>
       </c>
       <c r="R19" s="54" cm="1">
         <f t="array" ref="R19">INDEX(Calculation!AB22:AB$34,Calculation!$D$5)</f>
-        <v>0.54189944134078216</v>
+        <v>-0.32631578947368423</v>
       </c>
       <c r="S19" s="81" t="str">
         <f t="shared" si="3"/>
-        <v>▲</v>
+        <v>▼</v>
       </c>
       <c r="T19" s="56" cm="1">
         <f t="array" ref="T19">INDEX(Calculation!Q22:Q$34,Calculation!$D$5)</f>
-        <v>5353</v>
+        <v>8210</v>
       </c>
       <c r="V19" s="54" cm="1">
         <f t="array" ref="V19">INDEX(Calculation!Z22:Z$34,Calculation!$D$5)</f>
-        <v>0.13651804670912951</v>
+        <v>3.7901944002934345E-3</v>
       </c>
       <c r="W19" s="57">
         <f t="shared" si="4"/>
-        <v>0.13651804670912951</v>
+        <v>3.7901944002934345E-3</v>
       </c>
       <c r="Y19" s="54" cm="1">
         <f t="array" ref="Y19">INDEX(Calculation!AC22:AC$34,Calculation!$D$5)</f>
-        <v>3.1207859757272201E-2</v>
+        <v>2.4968789013732832E-2</v>
       </c>
       <c r="Z19" s="37" t="str">
         <f t="shared" si="5"/>
@@ -14672,69 +14671,69 @@
       </c>
       <c r="E20" s="60" t="str" cm="1">
         <f t="array" ref="E20">INDEX(Calculation!N23:N$34,Calculation!$D$5)</f>
-        <v>Aviatrr</v>
+        <v>Scrap</v>
       </c>
       <c r="F20" s="61" cm="1">
         <f t="array" ref="F20">INDEX(Calculation!O23:O$34,Calculation!$D$5)</f>
-        <v>8126</v>
+        <v>13307</v>
       </c>
       <c r="G20" s="60"/>
       <c r="H20" s="62" cm="1">
         <f t="array" ref="H20">INDEX(Calculation!X23:X$34,Calculation!$D$5)</f>
-        <v>-0.10811107452529908</v>
+        <v>9.730353756081471E-2</v>
       </c>
       <c r="I20" s="63">
         <f t="shared" si="0"/>
-        <v>-0.10811107452529908</v>
+        <v>9.730353756081471E-2</v>
       </c>
       <c r="J20" s="60"/>
       <c r="K20" s="62" cm="1">
         <f t="array" ref="K20">INDEX(Calculation!AA23:AA$34,Calculation!$D$5)</f>
-        <v>-5.9708400833140475E-2</v>
+        <v>-1.0484830458060678E-2</v>
       </c>
       <c r="L20" s="82" t="str">
         <f t="shared" si="1"/>
-        <v>▼</v>
+        <v/>
       </c>
       <c r="M20" s="61" cm="1">
         <f t="array" ref="M20">INDEX(Calculation!P23:P$34,Calculation!$D$5)</f>
-        <v>321</v>
+        <v>862</v>
       </c>
       <c r="N20" s="60"/>
       <c r="O20" s="62" cm="1">
         <f t="array" ref="O20">INDEX(Calculation!Y23:Y$34,Calculation!$D$5)</f>
-        <v>-0.43386243386243384</v>
+        <v>0.16172506738544473</v>
       </c>
       <c r="P20" s="63">
         <f t="shared" si="2"/>
-        <v>-0.43386243386243384</v>
+        <v>0.16172506738544473</v>
       </c>
       <c r="Q20" s="60"/>
       <c r="R20" s="62" cm="1">
         <f t="array" ref="R20">INDEX(Calculation!AB23:AB$34,Calculation!$D$5)</f>
-        <v>-0.42057761732851984</v>
+        <v>-4.7513812154696133E-2</v>
       </c>
       <c r="S20" s="82" t="str">
         <f t="shared" si="3"/>
-        <v>▼</v>
+        <v/>
       </c>
       <c r="T20" s="61" cm="1">
         <f t="array" ref="T20">INDEX(Calculation!Q23:Q$34,Calculation!$D$5)</f>
-        <v>6153</v>
+        <v>5279</v>
       </c>
       <c r="U20" s="60"/>
       <c r="V20" s="62" cm="1">
         <f t="array" ref="V20">INDEX(Calculation!Z23:Z$34,Calculation!$D$5)</f>
-        <v>3.2555797952676623E-2</v>
+        <v>-3.8608632307412127E-2</v>
       </c>
       <c r="W20" s="63">
         <f t="shared" si="4"/>
-        <v>3.2555797952676623E-2</v>
+        <v>-3.8608632307412127E-2</v>
       </c>
       <c r="X20" s="60"/>
       <c r="Y20" s="62" cm="1">
         <f t="array" ref="Y20">INDEX(Calculation!AC23:AC$34,Calculation!$D$5)</f>
-        <v>-0.16648604714169601</v>
+        <v>-0.12916529198284393</v>
       </c>
       <c r="Z20" s="64" t="str">
         <f t="shared" si="5"/>
@@ -15531,7 +15530,7 @@
       <c r="AE45" s="33"/>
     </row>
   </sheetData>
-  <sheetProtection insertHyperlinks="0"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="eNZ1UdSjAVyCkcfp40IoFqDLGBXmvNNHVdfulr4hEtzuGxJVAij2JnZ0hnLelRiMGovThS+WVSb95bQ8THfq9A==" saltValue="LRdPWMu1RLS91LASNCfIkg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <conditionalFormatting sqref="L11:L20">
     <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
       <formula>"▲"</formula>
@@ -15819,7 +15818,9 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="B1:P41"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
@@ -16522,7 +16523,7 @@
   <dimension ref="B2:AY44"/>
   <sheetViews>
     <sheetView topLeftCell="M1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Y27" sqref="Y27"/>
+      <selection activeCell="N20" sqref="N20 Q20 T20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -16599,7 +16600,7 @@
         <v>78</v>
       </c>
       <c r="D4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AE4" s="37"/>
       <c r="AF4" s="46"/>
@@ -16629,39 +16630,39 @@
       </c>
       <c r="O7" t="str">
         <f t="array" ref="O7">O8&amp;O9&amp;O10&amp;O11</f>
-        <v>2024SepActualRevenue</v>
+        <v>2024DecActualRevenue</v>
       </c>
       <c r="P7" t="str">
         <f t="array" ref="P7">P8&amp;P9&amp;P10&amp;P11</f>
-        <v>2024SepActualProfit</v>
+        <v>2024DecActualProfit</v>
       </c>
       <c r="Q7" t="str">
         <f t="array" ref="Q7">Q8&amp;Q9&amp;Q10&amp;Q11</f>
-        <v>2024SepActualCash</v>
+        <v>2024DecActualCash</v>
       </c>
       <c r="R7" t="str">
         <f t="array" ref="R7">R8&amp;R9&amp;R10&amp;R11</f>
-        <v>2023SepActualRevenue</v>
+        <v>2023DecActualRevenue</v>
       </c>
       <c r="S7" t="str">
         <f t="array" ref="S7">S8&amp;S9&amp;S10&amp;S11</f>
-        <v>2023SepActualProfit</v>
+        <v>2023DecActualProfit</v>
       </c>
       <c r="T7" t="str">
         <f t="array" ref="T7">T8&amp;T9&amp;T10&amp;T11</f>
-        <v>2023SepActualCash</v>
+        <v>2023DecActualCash</v>
       </c>
       <c r="U7" t="str">
         <f t="array" ref="U7">U8&amp;U9&amp;U10&amp;U11</f>
-        <v>2024SepBudgetRevenue</v>
+        <v>2024DecBudgetRevenue</v>
       </c>
       <c r="V7" t="str">
         <f t="array" ref="V7">V8&amp;V9&amp;V10&amp;V11</f>
-        <v>2024SepBudgetProfit</v>
+        <v>2024DecBudgetProfit</v>
       </c>
       <c r="W7" t="str">
         <f t="array" ref="W7">W8&amp;W9&amp;W10&amp;W11</f>
-        <v>2024SepBudgetCash</v>
+        <v>2024DecBudgetCash</v>
       </c>
     </row>
     <row r="8" spans="2:51" x14ac:dyDescent="0.25">
@@ -16669,7 +16670,7 @@
         <v>120</v>
       </c>
       <c r="D8">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="O8" s="46">
         <f>cur_year</f>
@@ -16726,39 +16727,39 @@
       </c>
       <c r="O9" t="str">
         <f t="shared" ref="O9:W9" si="0">cur_month</f>
-        <v>Sep</v>
+        <v>Dec</v>
       </c>
       <c r="P9" t="str">
         <f t="shared" si="0"/>
-        <v>Sep</v>
+        <v>Dec</v>
       </c>
       <c r="Q9" t="str">
         <f t="shared" si="0"/>
-        <v>Sep</v>
+        <v>Dec</v>
       </c>
       <c r="R9" t="str">
         <f t="shared" si="0"/>
-        <v>Sep</v>
+        <v>Dec</v>
       </c>
       <c r="S9" t="str">
         <f t="shared" si="0"/>
-        <v>Sep</v>
+        <v>Dec</v>
       </c>
       <c r="T9" t="str">
         <f t="shared" si="0"/>
-        <v>Sep</v>
+        <v>Dec</v>
       </c>
       <c r="U9" t="str">
         <f t="shared" si="0"/>
-        <v>Sep</v>
+        <v>Dec</v>
       </c>
       <c r="V9" t="str">
         <f t="shared" si="0"/>
-        <v>Sep</v>
+        <v>Dec</v>
       </c>
       <c r="W9" t="str">
         <f t="shared" si="0"/>
-        <v>Sep</v>
+        <v>Dec</v>
       </c>
       <c r="AH9" t="s">
         <v>110</v>
@@ -16800,11 +16801,11 @@
       </c>
       <c r="AP10" s="32" t="str" cm="1">
         <f t="array" ref="AP10">INDEX($G$13:$I$34,D8,D4)</f>
-        <v>Arcade</v>
+        <v>Infic</v>
       </c>
       <c r="AU10" t="str">
         <f>"Profit for "&amp;AP10</f>
-        <v>Profit for Arcade</v>
+        <v>Profit for Infic</v>
       </c>
     </row>
     <row r="11" spans="2:51" x14ac:dyDescent="0.25">
@@ -17063,111 +17064,111 @@
       </c>
       <c r="N14" s="46" t="str" cm="1">
         <f t="array" ref="N14">IF(G14&lt;&gt;"",INDEX(G14:I14,,$D$4),"")</f>
-        <v>Fightrr</v>
+        <v>Commuta</v>
       </c>
       <c r="O14" s="56">
         <f>IF($N14&lt;&gt;"",INDEX(Data!$B$9:$J$55,MATCH($N14,Data!$A$9:$A$51,0),MATCH(O$7,Data!$B$4:$AT$4,0)),"")</f>
-        <v>11649</v>
+        <v>6353</v>
       </c>
       <c r="P14" s="56">
         <f>IF($N14&lt;&gt;"",INDEX(Data!$B$9:$J$55,MATCH($N14,Data!$A$9:$A$51,0),MATCH(P$7,Data!$B$4:$AT$4,0)),"")</f>
-        <v>802</v>
+        <v>762</v>
       </c>
       <c r="Q14" s="56">
         <f>IF($N14&lt;&gt;"",INDEX(Data!$B$9:$J$55,MATCH($N14,Data!$A$9:$A$51,0),MATCH(Q$7,Data!$B$4:$AT$4,0)),"")</f>
-        <v>5956</v>
+        <v>7332</v>
       </c>
       <c r="R14" s="56">
         <f>IF($N14&lt;&gt;"",INDEX(Data!$B$9:$J$55,MATCH($N14,Data!$A$9:$A$51,0),MATCH(R$7,Data!$B$4:$AT$4,0)),"")</f>
-        <v>10414</v>
+        <v>5993</v>
       </c>
       <c r="S14" s="56">
         <f>IF($N14&lt;&gt;"",INDEX(Data!$B$9:$J$55,MATCH($N14,Data!$A$9:$A$51,0),MATCH(S$7,Data!$B$4:$AT$4,0)),"")</f>
-        <v>536</v>
+        <v>674</v>
       </c>
       <c r="T14" s="56">
         <f>IF($N14&lt;&gt;"",INDEX(Data!$B$9:$J$55,MATCH($N14,Data!$A$9:$A$51,0),MATCH(T$7,Data!$B$4:$AT$4,0)),"")</f>
-        <v>6713</v>
+        <v>7167</v>
       </c>
       <c r="U14" s="56">
         <f>IF($N14&lt;&gt;"",INDEX(Data!$B$9:$J$55,MATCH($N14,Data!$A$9:$A$51,0),MATCH(U$7,Data!$B$4:$AT$4,0)),"")</f>
-        <v>10593</v>
+        <v>5275</v>
       </c>
       <c r="V14" s="56">
         <f>IF($N14&lt;&gt;"",INDEX(Data!$B$9:$J$55,MATCH($N14,Data!$A$9:$A$51,0),MATCH(V$7,Data!$B$4:$AT$4,0)),"")</f>
-        <v>554</v>
+        <v>568</v>
       </c>
       <c r="W14" s="56">
         <f>IF($N14&lt;&gt;"",INDEX(Data!$B$9:$J$55,MATCH($N14,Data!$A$9:$A$51,0),MATCH(W$7,Data!$B$4:$AT$4,0)),"")</f>
-        <v>6803</v>
+        <v>7227</v>
       </c>
       <c r="X14" s="55">
         <f>IF($N14&lt;&gt;"",(O14-R14)/R14,"")</f>
-        <v>0.11859035913193777</v>
+        <v>6.0070081762055728E-2</v>
       </c>
       <c r="Y14" s="55">
         <f t="shared" ref="Y14:Z14" si="2">IF($N14&lt;&gt;"",(P14-S14)/S14,"")</f>
-        <v>0.4962686567164179</v>
+        <v>0.13056379821958458</v>
       </c>
       <c r="Z14" s="55">
         <f t="shared" si="2"/>
-        <v>-0.11276627439296887</v>
+        <v>2.3022185014650483E-2</v>
       </c>
       <c r="AA14" s="55">
         <f>IF($N14&lt;&gt;"",(O14-U14)/U14,"")</f>
-        <v>9.9688473520249218E-2</v>
+        <v>0.20436018957345972</v>
       </c>
       <c r="AB14" s="55">
         <f t="shared" ref="AB14:AC14" si="3">IF($N14&lt;&gt;"",(P14-V14)/V14,"")</f>
-        <v>0.44765342960288806</v>
+        <v>0.34154929577464788</v>
       </c>
       <c r="AC14" s="55">
         <f t="shared" si="3"/>
-        <v>-0.12450389534029105</v>
+        <v>1.4528850145288501E-2</v>
       </c>
       <c r="AE14" t="str">
         <f t="shared" ref="AE14:AE34" si="4">N14</f>
-        <v>Fightrr</v>
+        <v>Commuta</v>
       </c>
       <c r="AF14" s="57" cm="1">
         <f t="array" ref="AF14">IF(AE14="","",INDEX(AA14:AC14,$D$6)+(ROW()/10000000000)+N("No row function was used to achieve a unique value to sort"))</f>
-        <v>9.9688474920249223E-2</v>
+        <v>0.20436019097345973</v>
       </c>
       <c r="AG14" s="35"/>
       <c r="AH14" t="str">
         <f>INDEX($AE$14:$AE$34,MATCH(CHOOSE($D$7,LARGE($AF$14:$AF$34,$M14),SMALL($AF$14:$AF$34,$M14)),$AF$14:$AF$34,0))</f>
-        <v>Aviatrr</v>
+        <v>Strex</v>
       </c>
       <c r="AI14" s="73" cm="1">
         <f t="array" ref="AI14">INDEX($O$14:$Q$34,MATCH($AH14,$N$14:$N$34,0),$D$6)</f>
-        <v>8126</v>
+        <v>8152</v>
       </c>
       <c r="AJ14" s="73" cm="1">
         <f t="array" ref="AJ14">INDEX($U$14:$W$34,MATCH($AH14,$N$14:$N$34,0),$D$6)</f>
-        <v>8642</v>
+        <v>9698</v>
       </c>
       <c r="AK14" s="73">
         <f>MAX(AI14:AJ14)</f>
-        <v>8642</v>
+        <v>9698</v>
       </c>
       <c r="AL14" t="str" cm="1">
         <f t="array" ref="AL14">TEXT(INDEX($AA$14:$AC$34,MATCH(AH14,$AE$14:$AE$34,0),$D$6),"0%")&amp;" | "&amp;TEXT(AI14,"#,##0")</f>
-        <v>-6% | 8,126</v>
+        <v>-16% | 8,152</v>
       </c>
       <c r="AP14" t="s">
         <v>18</v>
       </c>
       <c r="AQ14" s="56" cm="1">
         <f t="array" ref="AQ14">INDEX(Data!$K$9:$AT$51,MATCH(Calculation!$AP$10,Data!$A$9:$A$51,0),MATCH(Calculation!AQ$12&amp;Calculation!$AP14&amp;Calculation!AQ$13,INDEX(Data!$K$5:$AT$5&amp;Data!$K$6:$AT$6&amp;Data!$K$7:$AT$7,),0))</f>
-        <v>17</v>
+        <v>82</v>
       </c>
       <c r="AR14" s="56" cm="1">
         <f t="array" ref="AR14">INDEX(Data!$K$9:$AT$51,MATCH(Calculation!$AP$10,Data!$A$9:$A$51,0),MATCH(Calculation!AR$12&amp;Calculation!$AP14&amp;Calculation!AR$13,INDEX(Data!$K$5:$AT$5&amp;Data!$K$6:$AT$6&amp;Data!$K$7:$AT$7,),0))</f>
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="AS14" s="56" cm="1">
         <f t="array" ref="AS14">INDEX(Data!$K$9:$AT$51,MATCH(Calculation!$AP$10,Data!$A$9:$A$51,0),MATCH(Calculation!AS$12&amp;Calculation!$AP14&amp;Calculation!AS$13,INDEX(Data!$K$5:$AT$5&amp;Data!$K$6:$AT$6&amp;Data!$K$7:$AT$7,),0))</f>
-        <v>22</v>
+        <v>71</v>
       </c>
       <c r="AU14" t="str">
         <f>LEFT(AP14,1)</f>
@@ -17175,15 +17176,15 @@
       </c>
       <c r="AV14">
         <f>IF(MATCH(cur_month,$AP$14:$AP$25,0)&gt;=ROWS(AP14:$AP$14),AQ14,NA())</f>
-        <v>17</v>
+        <v>82</v>
       </c>
       <c r="AW14" s="85">
         <f>IF($D$9,AR14,NA())</f>
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="AX14" s="85">
         <f>IF($D$10,AS14,NA())</f>
-        <v>22</v>
+        <v>71</v>
       </c>
       <c r="AY14" t="e">
         <f t="shared" ref="AY14:AY25" si="5">IF(cur_month=AP14,AQ14,NA())</f>
@@ -17215,111 +17216,111 @@
       </c>
       <c r="N15" s="46" t="str" cm="1">
         <f t="array" ref="N15">IF(G15&lt;&gt;"",INDEX(G15:I15,,$D$4),"")</f>
-        <v>Kryptis</v>
+        <v>Infic</v>
       </c>
       <c r="O15" s="56">
         <f>IF($N15&lt;&gt;"",INDEX(Data!$B$9:$J$55,MATCH($N15,Data!$A$9:$A$51,0),MATCH(O$7,Data!$B$4:$AT$4,0)),"")</f>
-        <v>7718</v>
+        <v>12373</v>
       </c>
       <c r="P15" s="56">
         <f>IF($N15&lt;&gt;"",INDEX(Data!$B$9:$J$55,MATCH($N15,Data!$A$9:$A$51,0),MATCH(P$7,Data!$B$4:$AT$4,0)),"")</f>
-        <v>876</v>
+        <v>408</v>
       </c>
       <c r="Q15" s="56">
         <f>IF($N15&lt;&gt;"",INDEX(Data!$B$9:$J$55,MATCH($N15,Data!$A$9:$A$51,0),MATCH(Q$7,Data!$B$4:$AT$4,0)),"")</f>
-        <v>8432</v>
+        <v>3054</v>
       </c>
       <c r="R15" s="56">
         <f>IF($N15&lt;&gt;"",INDEX(Data!$B$9:$J$55,MATCH($N15,Data!$A$9:$A$51,0),MATCH(R$7,Data!$B$4:$AT$4,0)),"")</f>
-        <v>7282</v>
+        <v>12398</v>
       </c>
       <c r="S15" s="56">
         <f>IF($N15&lt;&gt;"",INDEX(Data!$B$9:$J$55,MATCH($N15,Data!$A$9:$A$51,0),MATCH(S$7,Data!$B$4:$AT$4,0)),"")</f>
-        <v>775</v>
+        <v>341</v>
       </c>
       <c r="T15" s="56">
         <f>IF($N15&lt;&gt;"",INDEX(Data!$B$9:$J$55,MATCH($N15,Data!$A$9:$A$51,0),MATCH(T$7,Data!$B$4:$AT$4,0)),"")</f>
-        <v>8242</v>
+        <v>3033</v>
       </c>
       <c r="U15" s="56">
         <f>IF($N15&lt;&gt;"",INDEX(Data!$B$9:$J$55,MATCH($N15,Data!$A$9:$A$51,0),MATCH(U$7,Data!$B$4:$AT$4,0)),"")</f>
-        <v>6409</v>
+        <v>10472</v>
       </c>
       <c r="V15" s="56">
         <f>IF($N15&lt;&gt;"",INDEX(Data!$B$9:$J$55,MATCH($N15,Data!$A$9:$A$51,0),MATCH(V$7,Data!$B$4:$AT$4,0)),"")</f>
-        <v>654</v>
+        <v>461</v>
       </c>
       <c r="W15" s="56">
         <f>IF($N15&lt;&gt;"",INDEX(Data!$B$9:$J$55,MATCH($N15,Data!$A$9:$A$51,0),MATCH(W$7,Data!$B$4:$AT$4,0)),"")</f>
-        <v>8312</v>
+        <v>2910</v>
       </c>
       <c r="X15" s="55">
         <f t="shared" ref="X15:X34" si="7">IF($N15&lt;&gt;"",(O15-R15)/R15,"")</f>
-        <v>5.9873661082120298E-2</v>
+        <v>-2.0164542668172285E-3</v>
       </c>
       <c r="Y15" s="55">
         <f t="shared" ref="Y15:Y26" si="8">IF($N15&lt;&gt;"",(P15-S15)/S15,"")</f>
-        <v>0.13032258064516128</v>
+        <v>0.19648093841642228</v>
       </c>
       <c r="Z15" s="55">
         <f t="shared" ref="Z15:Z26" si="9">IF($N15&lt;&gt;"",(Q15-T15)/T15,"")</f>
-        <v>2.3052657122057753E-2</v>
+        <v>6.923837784371909E-3</v>
       </c>
       <c r="AA15" s="55">
         <f t="shared" ref="AA15:AA26" si="10">IF($N15&lt;&gt;"",(O15-U15)/U15,"")</f>
-        <v>0.20424403183023873</v>
+        <v>0.18153170359052712</v>
       </c>
       <c r="AB15" s="55">
         <f t="shared" ref="AB15:AB26" si="11">IF($N15&lt;&gt;"",(P15-V15)/V15,"")</f>
-        <v>0.33944954128440369</v>
+        <v>-0.11496746203904555</v>
       </c>
       <c r="AC15" s="55">
         <f t="shared" ref="AC15:AC26" si="12">IF($N15&lt;&gt;"",(Q15-W15)/W15,"")</f>
-        <v>1.4436958614051972E-2</v>
+        <v>4.9484536082474224E-2</v>
       </c>
       <c r="AE15" t="str">
         <f t="shared" si="4"/>
-        <v>Kryptis</v>
+        <v>Infic</v>
       </c>
       <c r="AF15" s="57" cm="1">
         <f t="array" ref="AF15">IF(AE15="","",INDEX(AA15:AC15,$D$6)+(ROW()/10000000000)+N("No row function was used to achieve a unique value to sort"))</f>
-        <v>0.20424403333023874</v>
+        <v>0.18153170509052713</v>
       </c>
       <c r="AG15" s="35"/>
       <c r="AH15" t="str">
         <f t="shared" ref="AH15:AH19" si="13">INDEX($AE$14:$AE$34,MATCH(CHOOSE($D$7,LARGE($AF$14:$AF$34,$M15),SMALL($AF$14:$AF$34,$M15)),$AF$14:$AF$34,0))</f>
-        <v>Hackrr</v>
+        <v>Amplefio</v>
       </c>
       <c r="AI15" s="73" cm="1">
         <f t="array" ref="AI15">INDEX($O$14:$Q$34,MATCH($AH15,$N$14:$N$34,0),$D$6)</f>
-        <v>18700.5</v>
+        <v>8250</v>
       </c>
       <c r="AJ15" s="73" cm="1">
         <f t="array" ref="AJ15">INDEX($U$14:$W$34,MATCH($AH15,$N$14:$N$34,0),$D$6)</f>
-        <v>19101.600000000002</v>
+        <v>8899</v>
       </c>
       <c r="AK15" s="73">
         <f t="shared" ref="AK15:AK19" si="14">MAX(AI15:AJ15)</f>
-        <v>19101.600000000002</v>
+        <v>8899</v>
       </c>
       <c r="AL15" t="str" cm="1">
         <f t="array" ref="AL15">TEXT(INDEX($AA$14:$AC$34,MATCH(AH15,$AE$14:$AE$34,0),$D$6),"0%")&amp;" | "&amp;TEXT(AI15,"#,##0")</f>
-        <v>-2% | 18,701</v>
+        <v>-7% | 8,250</v>
       </c>
       <c r="AP15" t="s">
         <v>19</v>
       </c>
       <c r="AQ15" s="56" cm="1">
         <f t="array" ref="AQ15">INDEX(Data!$K$9:$AT$51,MATCH(Calculation!$AP$10,Data!$A$9:$A$51,0),MATCH(Calculation!AQ$12&amp;Calculation!$AP15&amp;Calculation!AQ$13,INDEX(Data!$K$5:$AT$5&amp;Data!$K$6:$AT$6&amp;Data!$K$7:$AT$7,),0))</f>
-        <v>50</v>
+        <v>134</v>
       </c>
       <c r="AR15" s="56" cm="1">
         <f t="array" ref="AR15">INDEX(Data!$K$9:$AT$51,MATCH(Calculation!$AP$10,Data!$A$9:$A$51,0),MATCH(Calculation!AR$12&amp;Calculation!$AP15&amp;Calculation!AR$13,INDEX(Data!$K$5:$AT$5&amp;Data!$K$6:$AT$6&amp;Data!$K$7:$AT$7,),0))</f>
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="AS15" s="56" cm="1">
         <f t="array" ref="AS15">INDEX(Data!$K$9:$AT$51,MATCH(Calculation!$AP$10,Data!$A$9:$A$51,0),MATCH(Calculation!AS$12&amp;Calculation!$AP15&amp;Calculation!AS$13,INDEX(Data!$K$5:$AT$5&amp;Data!$K$6:$AT$6&amp;Data!$K$7:$AT$7,),0))</f>
-        <v>52</v>
+        <v>142</v>
       </c>
       <c r="AU15" t="str">
         <f t="shared" ref="AU15:AU25" si="15">LEFT(AP15,1)</f>
@@ -17327,15 +17328,15 @@
       </c>
       <c r="AV15">
         <f>IF(MATCH(cur_month,$AP$14:$AP$25,0)&gt;=ROWS(AP$14:$AP15),AQ15,NA())</f>
-        <v>50</v>
+        <v>134</v>
       </c>
       <c r="AW15" s="85">
         <f t="shared" ref="AW15:AW25" si="16">IF($D$9,AR15,NA())</f>
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="AX15" s="85">
         <f t="shared" ref="AX15:AX25" si="17">IF($D$10,AS15,NA())</f>
-        <v>52</v>
+        <v>142</v>
       </c>
       <c r="AY15" t="e">
         <f t="shared" si="5"/>
@@ -17367,111 +17368,111 @@
       </c>
       <c r="N16" s="46" t="str" cm="1">
         <f t="array" ref="N16">IF(G16&lt;&gt;"",INDEX(G16:I16,,$D$4),"")</f>
-        <v>Perino</v>
+        <v>Accord</v>
       </c>
       <c r="O16" s="56">
         <f>IF($N16&lt;&gt;"",INDEX(Data!$B$9:$J$55,MATCH($N16,Data!$A$9:$A$51,0),MATCH(O$7,Data!$B$4:$AT$4,0)),"")</f>
-        <v>15033</v>
+        <v>17760</v>
       </c>
       <c r="P16" s="56">
         <f>IF($N16&lt;&gt;"",INDEX(Data!$B$9:$J$55,MATCH($N16,Data!$A$9:$A$51,0),MATCH(P$7,Data!$B$4:$AT$4,0)),"")</f>
-        <v>469</v>
+        <v>800</v>
       </c>
       <c r="Q16" s="56">
         <f>IF($N16&lt;&gt;"",INDEX(Data!$B$9:$J$55,MATCH($N16,Data!$A$9:$A$51,0),MATCH(Q$7,Data!$B$4:$AT$4,0)),"")</f>
-        <v>3512</v>
+        <v>6488</v>
       </c>
       <c r="R16" s="56">
         <f>IF($N16&lt;&gt;"",INDEX(Data!$B$9:$J$55,MATCH($N16,Data!$A$9:$A$51,0),MATCH(R$7,Data!$B$4:$AT$4,0)),"")</f>
-        <v>15064</v>
+        <v>17025</v>
       </c>
       <c r="S16" s="56">
         <f>IF($N16&lt;&gt;"",INDEX(Data!$B$9:$J$55,MATCH($N16,Data!$A$9:$A$51,0),MATCH(S$7,Data!$B$4:$AT$4,0)),"")</f>
-        <v>392</v>
+        <v>568</v>
       </c>
       <c r="T16" s="56">
         <f>IF($N16&lt;&gt;"",INDEX(Data!$B$9:$J$55,MATCH($N16,Data!$A$9:$A$51,0),MATCH(T$7,Data!$B$4:$AT$4,0)),"")</f>
-        <v>3488</v>
+        <v>7469</v>
       </c>
       <c r="U16" s="56">
         <f>IF($N16&lt;&gt;"",INDEX(Data!$B$9:$J$55,MATCH($N16,Data!$A$9:$A$51,0),MATCH(U$7,Data!$B$4:$AT$4,0)),"")</f>
-        <v>12724</v>
+        <v>16854</v>
       </c>
       <c r="V16" s="56">
         <f>IF($N16&lt;&gt;"",INDEX(Data!$B$9:$J$55,MATCH($N16,Data!$A$9:$A$51,0),MATCH(V$7,Data!$B$4:$AT$4,0)),"")</f>
-        <v>530</v>
+        <v>572</v>
       </c>
       <c r="W16" s="56">
         <f>IF($N16&lt;&gt;"",INDEX(Data!$B$9:$J$55,MATCH($N16,Data!$A$9:$A$51,0),MATCH(W$7,Data!$B$4:$AT$4,0)),"")</f>
-        <v>3347</v>
+        <v>6611</v>
       </c>
       <c r="X16" s="55">
         <f t="shared" si="7"/>
-        <v>-2.0578863515666491E-3</v>
+        <v>4.3171806167400878E-2</v>
       </c>
       <c r="Y16" s="55">
         <f t="shared" si="8"/>
-        <v>0.19642857142857142</v>
+        <v>0.40845070422535212</v>
       </c>
       <c r="Z16" s="55">
         <f t="shared" si="9"/>
-        <v>6.8807339449541288E-3</v>
+        <v>-0.13134288392020352</v>
       </c>
       <c r="AA16" s="55">
         <f t="shared" si="10"/>
-        <v>0.18146809179503301</v>
+        <v>5.3755784976860094E-2</v>
       </c>
       <c r="AB16" s="55">
         <f t="shared" si="11"/>
-        <v>-0.11509433962264151</v>
+        <v>0.39860139860139859</v>
       </c>
       <c r="AC16" s="55">
         <f t="shared" si="12"/>
-        <v>4.9297878697340904E-2</v>
+        <v>-1.8605354711843897E-2</v>
       </c>
       <c r="AE16" t="str">
         <f t="shared" si="4"/>
-        <v>Perino</v>
+        <v>Accord</v>
       </c>
       <c r="AF16" s="57" cm="1">
         <f t="array" ref="AF16">IF(AE16="","",INDEX(AA16:AC16,$D$6)+(ROW()/10000000000)+N("No row function was used to achieve a unique value to sort"))</f>
-        <v>0.181468093395033</v>
+        <v>5.3755786576860094E-2</v>
       </c>
       <c r="AG16" s="35"/>
       <c r="AH16" t="str">
         <f t="shared" si="13"/>
-        <v>Baden</v>
+        <v>Atmos</v>
       </c>
       <c r="AI16" s="73" cm="1">
         <f t="array" ref="AI16">INDEX($O$14:$Q$34,MATCH($AH16,$N$14:$N$34,0),$D$6)</f>
-        <v>35980</v>
+        <v>10675</v>
       </c>
       <c r="AJ16" s="73" cm="1">
         <f t="array" ref="AJ16">INDEX($U$14:$W$34,MATCH($AH16,$N$14:$N$34,0),$D$6)</f>
-        <v>36362</v>
+        <v>11178</v>
       </c>
       <c r="AK16" s="73">
         <f t="shared" si="14"/>
-        <v>36362</v>
+        <v>11178</v>
       </c>
       <c r="AL16" t="str" cm="1">
         <f t="array" ref="AL16">TEXT(INDEX($AA$14:$AC$34,MATCH(AH16,$AE$14:$AE$34,0),$D$6),"0%")&amp;" | "&amp;TEXT(AI16,"#,##0")</f>
-        <v>-1% | 35,980</v>
+        <v>-4% | 10,675</v>
       </c>
       <c r="AP16" t="s">
         <v>20</v>
       </c>
       <c r="AQ16" s="56" cm="1">
         <f t="array" ref="AQ16">INDEX(Data!$K$9:$AT$51,MATCH(Calculation!$AP$10,Data!$A$9:$A$51,0),MATCH(Calculation!AQ$12&amp;Calculation!$AP16&amp;Calculation!AQ$13,INDEX(Data!$K$5:$AT$5&amp;Data!$K$6:$AT$6&amp;Data!$K$7:$AT$7,),0))</f>
-        <v>67</v>
+        <v>187</v>
       </c>
       <c r="AR16" s="56" cm="1">
         <f t="array" ref="AR16">INDEX(Data!$K$9:$AT$51,MATCH(Calculation!$AP$10,Data!$A$9:$A$51,0),MATCH(Calculation!AR$12&amp;Calculation!$AP16&amp;Calculation!AR$13,INDEX(Data!$K$5:$AT$5&amp;Data!$K$6:$AT$6&amp;Data!$K$7:$AT$7,),0))</f>
-        <v>27</v>
+        <v>89</v>
       </c>
       <c r="AS16" s="56" cm="1">
         <f t="array" ref="AS16">INDEX(Data!$K$9:$AT$51,MATCH(Calculation!$AP$10,Data!$A$9:$A$51,0),MATCH(Calculation!AS$12&amp;Calculation!$AP16&amp;Calculation!AS$13,INDEX(Data!$K$5:$AT$5&amp;Data!$K$6:$AT$6&amp;Data!$K$7:$AT$7,),0))</f>
-        <v>90</v>
+        <v>247</v>
       </c>
       <c r="AU16" t="str">
         <f t="shared" si="15"/>
@@ -17479,15 +17480,15 @@
       </c>
       <c r="AV16">
         <f>IF(MATCH(cur_month,$AP$14:$AP$25,0)&gt;=ROWS(AP$14:$AP16),AQ16,NA())</f>
-        <v>67</v>
+        <v>187</v>
       </c>
       <c r="AW16" s="85">
         <f t="shared" si="16"/>
-        <v>27</v>
+        <v>89</v>
       </c>
       <c r="AX16" s="85">
         <f t="shared" si="17"/>
-        <v>90</v>
+        <v>247</v>
       </c>
       <c r="AY16" t="e">
         <f t="shared" si="5"/>
@@ -17513,111 +17514,111 @@
       </c>
       <c r="N17" s="46" t="str" cm="1">
         <f t="array" ref="N17">IF(G17&lt;&gt;"",INDEX(G17:I17,,$D$4),"")</f>
-        <v>Five Labs</v>
+        <v>Misty Wash</v>
       </c>
       <c r="O17" s="56">
         <f>IF($N17&lt;&gt;"",INDEX(Data!$B$9:$J$55,MATCH($N17,Data!$A$9:$A$51,0),MATCH(O$7,Data!$B$4:$AT$4,0)),"")</f>
-        <v>21579</v>
+        <v>30399.599999999999</v>
       </c>
       <c r="P17" s="56">
         <f>IF($N17&lt;&gt;"",INDEX(Data!$B$9:$J$55,MATCH($N17,Data!$A$9:$A$51,0),MATCH(P$7,Data!$B$4:$AT$4,0)),"")</f>
-        <v>920</v>
+        <v>786.8</v>
       </c>
       <c r="Q17" s="56">
         <f>IF($N17&lt;&gt;"",INDEX(Data!$B$9:$J$55,MATCH($N17,Data!$A$9:$A$51,0),MATCH(Q$7,Data!$B$4:$AT$4,0)),"")</f>
-        <v>7461</v>
+        <v>12308.8</v>
       </c>
       <c r="R17" s="56">
         <f>IF($N17&lt;&gt;"",INDEX(Data!$B$9:$J$55,MATCH($N17,Data!$A$9:$A$51,0),MATCH(R$7,Data!$B$4:$AT$4,0)),"")</f>
-        <v>20686</v>
+        <v>29531.599999999999</v>
       </c>
       <c r="S17" s="56">
         <f>IF($N17&lt;&gt;"",INDEX(Data!$B$9:$J$55,MATCH($N17,Data!$A$9:$A$51,0),MATCH(S$7,Data!$B$4:$AT$4,0)),"")</f>
-        <v>653</v>
+        <v>786.8</v>
       </c>
       <c r="T17" s="56">
         <f>IF($N17&lt;&gt;"",INDEX(Data!$B$9:$J$55,MATCH($N17,Data!$A$9:$A$51,0),MATCH(T$7,Data!$B$4:$AT$4,0)),"")</f>
-        <v>8589</v>
+        <v>13941.199999999999</v>
       </c>
       <c r="U17" s="56">
         <f>IF($N17&lt;&gt;"",INDEX(Data!$B$9:$J$55,MATCH($N17,Data!$A$9:$A$51,0),MATCH(U$7,Data!$B$4:$AT$4,0)),"")</f>
-        <v>20478</v>
+        <v>30237.199999999997</v>
       </c>
       <c r="V17" s="56">
         <f>IF($N17&lt;&gt;"",INDEX(Data!$B$9:$J$55,MATCH($N17,Data!$A$9:$A$51,0),MATCH(V$7,Data!$B$4:$AT$4,0)),"")</f>
-        <v>658</v>
+        <v>932.4</v>
       </c>
       <c r="W17" s="56">
         <f>IF($N17&lt;&gt;"",INDEX(Data!$B$9:$J$55,MATCH($N17,Data!$A$9:$A$51,0),MATCH(W$7,Data!$B$4:$AT$4,0)),"")</f>
-        <v>7602</v>
+        <v>13381.199999999999</v>
       </c>
       <c r="X17" s="55">
         <f t="shared" si="7"/>
-        <v>4.3169293241806052E-2</v>
+        <v>2.9392244240068269E-2</v>
       </c>
       <c r="Y17" s="55">
         <f t="shared" si="8"/>
-        <v>0.40888208269525267</v>
+        <v>0</v>
       </c>
       <c r="Z17" s="55">
         <f t="shared" si="9"/>
-        <v>-0.13133077191756898</v>
+        <v>-0.11709178549909618</v>
       </c>
       <c r="AA17" s="55">
         <f t="shared" si="10"/>
-        <v>5.3765016114854965E-2</v>
+        <v>5.3708676729327274E-3</v>
       </c>
       <c r="AB17" s="55">
         <f t="shared" si="11"/>
-        <v>0.3981762917933131</v>
+        <v>-0.15615615615615619</v>
       </c>
       <c r="AC17" s="55">
         <f t="shared" si="12"/>
-        <v>-1.8547750591949488E-2</v>
+        <v>-8.014228918183719E-2</v>
       </c>
       <c r="AE17" t="str">
         <f t="shared" si="4"/>
-        <v>Five Labs</v>
+        <v>Misty Wash</v>
       </c>
       <c r="AF17" s="57" cm="1">
         <f t="array" ref="AF17">IF(AE17="","",INDEX(AA17:AC17,$D$6)+(ROW()/10000000000)+N("No row function was used to achieve a unique value to sort"))</f>
-        <v>5.3765017814854967E-2</v>
+        <v>5.3708693729327276E-3</v>
       </c>
       <c r="AG17" s="35"/>
       <c r="AH17" t="str">
         <f t="shared" si="13"/>
-        <v>Five Labs</v>
+        <v>Scrap</v>
       </c>
       <c r="AI17" s="73" cm="1">
         <f t="array" ref="AI17">INDEX($O$14:$Q$34,MATCH($AH17,$N$14:$N$34,0),$D$6)</f>
-        <v>21579</v>
+        <v>13307</v>
       </c>
       <c r="AJ17" s="73" cm="1">
         <f t="array" ref="AJ17">INDEX($U$14:$W$34,MATCH($AH17,$N$14:$N$34,0),$D$6)</f>
-        <v>20478</v>
+        <v>13448</v>
       </c>
       <c r="AK17" s="73">
         <f t="shared" si="14"/>
-        <v>21579</v>
+        <v>13448</v>
       </c>
       <c r="AL17" t="str" cm="1">
         <f t="array" ref="AL17">TEXT(INDEX($AA$14:$AC$34,MATCH(AH17,$AE$14:$AE$34,0),$D$6),"0%")&amp;" | "&amp;TEXT(AI17,"#,##0")</f>
-        <v>5% | 21,579</v>
+        <v>-1% | 13,307</v>
       </c>
       <c r="AP17" t="s">
         <v>21</v>
       </c>
       <c r="AQ17" s="56" cm="1">
         <f t="array" ref="AQ17">INDEX(Data!$K$9:$AT$51,MATCH(Calculation!$AP$10,Data!$A$9:$A$51,0),MATCH(Calculation!AQ$12&amp;Calculation!$AP17&amp;Calculation!AQ$13,INDEX(Data!$K$5:$AT$5&amp;Data!$K$6:$AT$6&amp;Data!$K$7:$AT$7,),0))</f>
-        <v>80</v>
+        <v>244</v>
       </c>
       <c r="AR17" s="56" cm="1">
         <f t="array" ref="AR17">INDEX(Data!$K$9:$AT$51,MATCH(Calculation!$AP$10,Data!$A$9:$A$51,0),MATCH(Calculation!AR$12&amp;Calculation!$AP17&amp;Calculation!AR$13,INDEX(Data!$K$5:$AT$5&amp;Data!$K$6:$AT$6&amp;Data!$K$7:$AT$7,),0))</f>
-        <v>105</v>
+        <v>179</v>
       </c>
       <c r="AS17" s="56" cm="1">
         <f t="array" ref="AS17">INDEX(Data!$K$9:$AT$51,MATCH(Calculation!$AP$10,Data!$A$9:$A$51,0),MATCH(Calculation!AS$12&amp;Calculation!$AP17&amp;Calculation!AS$13,INDEX(Data!$K$5:$AT$5&amp;Data!$K$6:$AT$6&amp;Data!$K$7:$AT$7,),0))</f>
-        <v>150</v>
+        <v>307</v>
       </c>
       <c r="AU17" t="str">
         <f t="shared" si="15"/>
@@ -17625,15 +17626,15 @@
       </c>
       <c r="AV17">
         <f>IF(MATCH(cur_month,$AP$14:$AP$25,0)&gt;=ROWS(AP$14:$AP17),AQ17,NA())</f>
-        <v>80</v>
+        <v>244</v>
       </c>
       <c r="AW17" s="85">
         <f t="shared" si="16"/>
-        <v>105</v>
+        <v>179</v>
       </c>
       <c r="AX17" s="85">
         <f t="shared" si="17"/>
-        <v>150</v>
+        <v>307</v>
       </c>
       <c r="AY17" t="e">
         <f t="shared" si="5"/>
@@ -17659,111 +17660,111 @@
       </c>
       <c r="N18" s="46" t="str" cm="1">
         <f t="array" ref="N18">IF(G18&lt;&gt;"",INDEX(G18:I18,,$D$4),"")</f>
-        <v>Twistrr</v>
+        <v>Twenty20</v>
       </c>
       <c r="O18" s="56">
         <f>IF($N18&lt;&gt;"",INDEX(Data!$B$9:$J$55,MATCH($N18,Data!$A$9:$A$51,0),MATCH(O$7,Data!$B$4:$AT$4,0)),"")</f>
-        <v>27210.600000000002</v>
+        <v>20400</v>
       </c>
       <c r="P18" s="56">
         <f>IF($N18&lt;&gt;"",INDEX(Data!$B$9:$J$55,MATCH($N18,Data!$A$9:$A$51,0),MATCH(P$7,Data!$B$4:$AT$4,0)),"")</f>
-        <v>2903.4</v>
+        <v>614.40000000000009</v>
       </c>
       <c r="Q18" s="56">
         <f>IF($N18&lt;&gt;"",INDEX(Data!$B$9:$J$55,MATCH($N18,Data!$A$9:$A$51,0),MATCH(Q$7,Data!$B$4:$AT$4,0)),"")</f>
-        <v>10490.4</v>
+        <v>15171.2</v>
       </c>
       <c r="R18" s="56">
         <f>IF($N18&lt;&gt;"",INDEX(Data!$B$9:$J$55,MATCH($N18,Data!$A$9:$A$51,0),MATCH(R$7,Data!$B$4:$AT$4,0)),"")</f>
-        <v>25448.400000000001</v>
+        <v>22224</v>
       </c>
       <c r="S18" s="56">
         <f>IF($N18&lt;&gt;"",INDEX(Data!$B$9:$J$55,MATCH($N18,Data!$A$9:$A$51,0),MATCH(S$7,Data!$B$4:$AT$4,0)),"")</f>
-        <v>2160</v>
+        <v>988.80000000000007</v>
       </c>
       <c r="T18" s="56">
         <f>IF($N18&lt;&gt;"",INDEX(Data!$B$9:$J$55,MATCH($N18,Data!$A$9:$A$51,0),MATCH(T$7,Data!$B$4:$AT$4,0)),"")</f>
-        <v>11181.6</v>
+        <v>16019.2</v>
       </c>
       <c r="U18" s="56">
         <f>IF($N18&lt;&gt;"",INDEX(Data!$B$9:$J$55,MATCH($N18,Data!$A$9:$A$51,0),MATCH(U$7,Data!$B$4:$AT$4,0)),"")</f>
-        <v>24219</v>
+        <v>18476.8</v>
       </c>
       <c r="V18" s="56">
         <f>IF($N18&lt;&gt;"",INDEX(Data!$B$9:$J$55,MATCH($N18,Data!$A$9:$A$51,0),MATCH(V$7,Data!$B$4:$AT$4,0)),"")</f>
-        <v>2520</v>
+        <v>1120</v>
       </c>
       <c r="W18" s="56">
         <f>IF($N18&lt;&gt;"",INDEX(Data!$B$9:$J$55,MATCH($N18,Data!$A$9:$A$51,0),MATCH(W$7,Data!$B$4:$AT$4,0)),"")</f>
-        <v>10458</v>
+        <v>14230.400000000001</v>
       </c>
       <c r="X18" s="55">
         <f t="shared" si="7"/>
-        <v>6.9246003678030868E-2</v>
+        <v>-8.2073434125269976E-2</v>
       </c>
       <c r="Y18" s="55">
         <f t="shared" si="8"/>
-        <v>0.34416666666666673</v>
+        <v>-0.37864077669902907</v>
       </c>
       <c r="Z18" s="55">
         <f t="shared" si="9"/>
-        <v>-6.1815840309079266E-2</v>
+        <v>-5.2936476228525764E-2</v>
       </c>
       <c r="AA18" s="55">
         <f t="shared" si="10"/>
-        <v>0.12352285395763665</v>
+        <v>0.10408728784205061</v>
       </c>
       <c r="AB18" s="55">
         <f t="shared" si="11"/>
-        <v>0.15214285714285719</v>
+        <v>-0.45142857142857135</v>
       </c>
       <c r="AC18" s="55">
         <f t="shared" si="12"/>
-        <v>3.0981067125645089E-3</v>
+        <v>6.6111985608275178E-2</v>
       </c>
       <c r="AE18" t="str">
         <f t="shared" si="4"/>
-        <v>Twistrr</v>
+        <v>Twenty20</v>
       </c>
       <c r="AF18" s="57" cm="1">
         <f t="array" ref="AF18">IF(AE18="","",INDEX(AA18:AC18,$D$6)+(ROW()/10000000000)+N("No row function was used to achieve a unique value to sort"))</f>
-        <v>0.12352285575763665</v>
+        <v>0.10408728964205061</v>
       </c>
       <c r="AG18" s="35"/>
       <c r="AH18" t="str">
         <f t="shared" si="13"/>
-        <v>Pes</v>
+        <v>Misty Wash</v>
       </c>
       <c r="AI18" s="73" cm="1">
         <f t="array" ref="AI18">INDEX($O$14:$Q$34,MATCH($AH18,$N$14:$N$34,0),$D$6)</f>
-        <v>45315.9</v>
+        <v>30399.599999999999</v>
       </c>
       <c r="AJ18" s="73" cm="1">
         <f t="array" ref="AJ18">INDEX($U$14:$W$34,MATCH($AH18,$N$14:$N$34,0),$D$6)</f>
-        <v>43003.8</v>
+        <v>30237.199999999997</v>
       </c>
       <c r="AK18" s="73">
         <f t="shared" si="14"/>
-        <v>45315.9</v>
+        <v>30399.599999999999</v>
       </c>
       <c r="AL18" t="str" cm="1">
         <f t="array" ref="AL18">TEXT(INDEX($AA$14:$AC$34,MATCH(AH18,$AE$14:$AE$34,0),$D$6),"0%")&amp;" | "&amp;TEXT(AI18,"#,##0")</f>
-        <v>5% | 45,316</v>
+        <v>1% | 30,400</v>
       </c>
       <c r="AP18" t="s">
         <v>22</v>
       </c>
       <c r="AQ18" s="56" cm="1">
         <f t="array" ref="AQ18">INDEX(Data!$K$9:$AT$51,MATCH(Calculation!$AP$10,Data!$A$9:$A$51,0),MATCH(Calculation!AQ$12&amp;Calculation!$AP18&amp;Calculation!AQ$13,INDEX(Data!$K$5:$AT$5&amp;Data!$K$6:$AT$6&amp;Data!$K$7:$AT$7,),0))</f>
-        <v>122</v>
+        <v>338</v>
       </c>
       <c r="AR18" s="56" cm="1">
         <f t="array" ref="AR18">INDEX(Data!$K$9:$AT$51,MATCH(Calculation!$AP$10,Data!$A$9:$A$51,0),MATCH(Calculation!AR$12&amp;Calculation!$AP18&amp;Calculation!AR$13,INDEX(Data!$K$5:$AT$5&amp;Data!$K$6:$AT$6&amp;Data!$K$7:$AT$7,),0))</f>
-        <v>218</v>
+        <v>234</v>
       </c>
       <c r="AS18" s="56" cm="1">
         <f t="array" ref="AS18">INDEX(Data!$K$9:$AT$51,MATCH(Calculation!$AP$10,Data!$A$9:$A$51,0),MATCH(Calculation!AS$12&amp;Calculation!$AP18&amp;Calculation!AS$13,INDEX(Data!$K$5:$AT$5&amp;Data!$K$6:$AT$6&amp;Data!$K$7:$AT$7,),0))</f>
-        <v>258</v>
+        <v>395</v>
       </c>
       <c r="AU18" t="str">
         <f t="shared" si="15"/>
@@ -17771,15 +17772,15 @@
       </c>
       <c r="AV18">
         <f>IF(MATCH(cur_month,$AP$14:$AP$25,0)&gt;=ROWS(AP$14:$AP18),AQ18,NA())</f>
-        <v>122</v>
+        <v>338</v>
       </c>
       <c r="AW18" s="85">
         <f t="shared" si="16"/>
-        <v>218</v>
+        <v>234</v>
       </c>
       <c r="AX18" s="85">
         <f t="shared" si="17"/>
-        <v>258</v>
+        <v>395</v>
       </c>
       <c r="AY18" t="e">
         <f t="shared" si="5"/>
@@ -17805,111 +17806,111 @@
       </c>
       <c r="N19" s="46" t="str" cm="1">
         <f t="array" ref="N19">IF(G19&lt;&gt;"",INDEX(G19:I19,,$D$4),"")</f>
-        <v>Hackrr</v>
+        <v>Tanox</v>
       </c>
       <c r="O19" s="56">
         <f>IF($N19&lt;&gt;"",INDEX(Data!$B$9:$J$55,MATCH($N19,Data!$A$9:$A$51,0),MATCH(O$7,Data!$B$4:$AT$4,0)),"")</f>
-        <v>18700.5</v>
+        <v>21088</v>
       </c>
       <c r="P19" s="56">
         <f>IF($N19&lt;&gt;"",INDEX(Data!$B$9:$J$55,MATCH($N19,Data!$A$9:$A$51,0),MATCH(P$7,Data!$B$4:$AT$4,0)),"")</f>
-        <v>984.90000000000009</v>
+        <v>1264</v>
       </c>
       <c r="Q19" s="56">
         <f>IF($N19&lt;&gt;"",INDEX(Data!$B$9:$J$55,MATCH($N19,Data!$A$9:$A$51,0),MATCH(Q$7,Data!$B$4:$AT$4,0)),"")</f>
-        <v>12654.6</v>
+        <v>4828</v>
       </c>
       <c r="R19" s="56">
         <f>IF($N19&lt;&gt;"",INDEX(Data!$B$9:$J$55,MATCH($N19,Data!$A$9:$A$51,0),MATCH(R$7,Data!$B$4:$AT$4,0)),"")</f>
-        <v>18471.600000000002</v>
+        <v>19736</v>
       </c>
       <c r="S19" s="56">
         <f>IF($N19&lt;&gt;"",INDEX(Data!$B$9:$J$55,MATCH($N19,Data!$A$9:$A$51,0),MATCH(S$7,Data!$B$4:$AT$4,0)),"")</f>
-        <v>663.6</v>
+        <v>932</v>
       </c>
       <c r="T19" s="56">
         <f>IF($N19&lt;&gt;"",INDEX(Data!$B$9:$J$55,MATCH($N19,Data!$A$9:$A$51,0),MATCH(T$7,Data!$B$4:$AT$4,0)),"")</f>
-        <v>13127.1</v>
+        <v>5940</v>
       </c>
       <c r="U19" s="56">
         <f>IF($N19&lt;&gt;"",INDEX(Data!$B$9:$J$55,MATCH($N19,Data!$A$9:$A$51,0),MATCH(U$7,Data!$B$4:$AT$4,0)),"")</f>
-        <v>19101.600000000002</v>
+        <v>19156</v>
       </c>
       <c r="V19" s="56">
         <f>IF($N19&lt;&gt;"",INDEX(Data!$B$9:$J$55,MATCH($N19,Data!$A$9:$A$51,0),MATCH(V$7,Data!$B$4:$AT$4,0)),"")</f>
-        <v>1302</v>
+        <v>860</v>
       </c>
       <c r="W19" s="56">
         <f>IF($N19&lt;&gt;"",INDEX(Data!$B$9:$J$55,MATCH($N19,Data!$A$9:$A$51,0),MATCH(W$7,Data!$B$4:$AT$4,0)),"")</f>
-        <v>12188.4</v>
+        <v>7744</v>
       </c>
       <c r="X19" s="55">
         <f t="shared" si="7"/>
-        <v>1.2391996361982599E-2</v>
+        <v>6.8504256181597084E-2</v>
       </c>
       <c r="Y19" s="55">
         <f t="shared" si="8"/>
-        <v>0.4841772151898735</v>
+        <v>0.35622317596566522</v>
       </c>
       <c r="Z19" s="55">
         <f t="shared" si="9"/>
-        <v>-3.5994240921452564E-2</v>
+        <v>-0.18720538720538721</v>
       </c>
       <c r="AA19" s="55">
         <f t="shared" si="10"/>
-        <v>-2.0998240985048485E-2</v>
+        <v>0.10085612862810607</v>
       </c>
       <c r="AB19" s="55">
         <f t="shared" si="11"/>
-        <v>-0.24354838709677412</v>
+        <v>0.4697674418604651</v>
       </c>
       <c r="AC19" s="55">
         <f t="shared" si="12"/>
-        <v>3.8249483115093103E-2</v>
+        <v>-0.37654958677685951</v>
       </c>
       <c r="AE19" t="str">
         <f t="shared" si="4"/>
-        <v>Hackrr</v>
+        <v>Tanox</v>
       </c>
       <c r="AF19" s="57" cm="1">
         <f t="array" ref="AF19">IF(AE19="","",INDEX(AA19:AC19,$D$6)+(ROW()/10000000000)+N("No row function was used to achieve a unique value to sort"))</f>
-        <v>-2.0998239085048484E-2</v>
+        <v>0.10085613052810607</v>
       </c>
       <c r="AG19" s="35"/>
       <c r="AH19" t="str">
         <f t="shared" si="13"/>
-        <v>Fightrr</v>
+        <v>Accord</v>
       </c>
       <c r="AI19" s="73" cm="1">
         <f t="array" ref="AI19">INDEX($O$14:$Q$34,MATCH($AH19,$N$14:$N$34,0),$D$6)</f>
-        <v>11649</v>
+        <v>17760</v>
       </c>
       <c r="AJ19" s="73" cm="1">
         <f t="array" ref="AJ19">INDEX($U$14:$W$34,MATCH($AH19,$N$14:$N$34,0),$D$6)</f>
-        <v>10593</v>
+        <v>16854</v>
       </c>
       <c r="AK19" s="73">
         <f t="shared" si="14"/>
-        <v>11649</v>
+        <v>17760</v>
       </c>
       <c r="AL19" t="str" cm="1">
         <f t="array" ref="AL19">TEXT(INDEX($AA$14:$AC$34,MATCH(AH19,$AE$14:$AE$34,0),$D$6),"0%")&amp;" | "&amp;TEXT(AI19,"#,##0")</f>
-        <v>10% | 11,649</v>
+        <v>5% | 17,760</v>
       </c>
       <c r="AP19" t="s">
         <v>17</v>
       </c>
       <c r="AQ19" s="56" cm="1">
         <f t="array" ref="AQ19">INDEX(Data!$K$9:$AT$51,MATCH(Calculation!$AP$10,Data!$A$9:$A$51,0),MATCH(Calculation!AQ$12&amp;Calculation!$AP19&amp;Calculation!AQ$13,INDEX(Data!$K$5:$AT$5&amp;Data!$K$6:$AT$6&amp;Data!$K$7:$AT$7,),0))</f>
-        <v>192</v>
+        <v>408</v>
       </c>
       <c r="AR19" s="56" cm="1">
         <f t="array" ref="AR19">INDEX(Data!$K$9:$AT$51,MATCH(Calculation!$AP$10,Data!$A$9:$A$51,0),MATCH(Calculation!AR$12&amp;Calculation!$AP19&amp;Calculation!AR$13,INDEX(Data!$K$5:$AT$5&amp;Data!$K$6:$AT$6&amp;Data!$K$7:$AT$7,),0))</f>
-        <v>309</v>
+        <v>341</v>
       </c>
       <c r="AS19" s="56" cm="1">
         <f t="array" ref="AS19">INDEX(Data!$K$9:$AT$51,MATCH(Calculation!$AP$10,Data!$A$9:$A$51,0),MATCH(Calculation!AS$12&amp;Calculation!$AP19&amp;Calculation!AS$13,INDEX(Data!$K$5:$AT$5&amp;Data!$K$6:$AT$6&amp;Data!$K$7:$AT$7,),0))</f>
-        <v>350</v>
+        <v>461</v>
       </c>
       <c r="AU19" t="str">
         <f t="shared" si="15"/>
@@ -17917,15 +17918,15 @@
       </c>
       <c r="AV19">
         <f>IF(MATCH(cur_month,$AP$14:$AP$25,0)&gt;=ROWS(AP$14:$AP19),AQ19,NA())</f>
-        <v>192</v>
+        <v>408</v>
       </c>
       <c r="AW19" s="85">
         <f t="shared" si="16"/>
-        <v>309</v>
+        <v>341</v>
       </c>
       <c r="AX19" s="85">
         <f t="shared" si="17"/>
-        <v>350</v>
+        <v>461</v>
       </c>
       <c r="AY19" t="e">
         <f t="shared" si="5"/>
@@ -17951,47 +17952,47 @@
       </c>
       <c r="N20" s="46" t="str" cm="1">
         <f t="array" ref="N20">IF(G20&lt;&gt;"",INDEX(G20:I20,,$D$4),"")</f>
-        <v>Pes</v>
+        <v>Minor Liar</v>
       </c>
       <c r="O20" s="56">
         <f>IF($N20&lt;&gt;"",INDEX(Data!$B$9:$J$55,MATCH($N20,Data!$A$9:$A$51,0),MATCH(O$7,Data!$B$4:$AT$4,0)),"")</f>
-        <v>45315.9</v>
+        <v>23736.9</v>
       </c>
       <c r="P20" s="56">
         <f>IF($N20&lt;&gt;"",INDEX(Data!$B$9:$J$55,MATCH($N20,Data!$A$9:$A$51,0),MATCH(P$7,Data!$B$4:$AT$4,0)),"")</f>
-        <v>1932</v>
+        <v>1012.0000000000001</v>
       </c>
       <c r="Q20" s="56">
         <f>IF($N20&lt;&gt;"",INDEX(Data!$B$9:$J$55,MATCH($N20,Data!$A$9:$A$51,0),MATCH(Q$7,Data!$B$4:$AT$4,0)),"")</f>
-        <v>15668.1</v>
+        <v>8207.1</v>
       </c>
       <c r="R20" s="56">
         <f>IF($N20&lt;&gt;"",INDEX(Data!$B$9:$J$55,MATCH($N20,Data!$A$9:$A$51,0),MATCH(R$7,Data!$B$4:$AT$4,0)),"")</f>
-        <v>43440.6</v>
+        <v>22754.600000000002</v>
       </c>
       <c r="S20" s="56">
         <f>IF($N20&lt;&gt;"",INDEX(Data!$B$9:$J$55,MATCH($N20,Data!$A$9:$A$51,0),MATCH(S$7,Data!$B$4:$AT$4,0)),"")</f>
-        <v>1371.3</v>
+        <v>718.30000000000007</v>
       </c>
       <c r="T20" s="56">
         <f>IF($N20&lt;&gt;"",INDEX(Data!$B$9:$J$55,MATCH($N20,Data!$A$9:$A$51,0),MATCH(T$7,Data!$B$4:$AT$4,0)),"")</f>
-        <v>18036.900000000001</v>
+        <v>9447.9000000000015</v>
       </c>
       <c r="U20" s="56">
         <f>IF($N20&lt;&gt;"",INDEX(Data!$B$9:$J$55,MATCH($N20,Data!$A$9:$A$51,0),MATCH(U$7,Data!$B$4:$AT$4,0)),"")</f>
-        <v>43003.8</v>
+        <v>22525.800000000003</v>
       </c>
       <c r="V20" s="56">
         <f>IF($N20&lt;&gt;"",INDEX(Data!$B$9:$J$55,MATCH($N20,Data!$A$9:$A$51,0),MATCH(V$7,Data!$B$4:$AT$4,0)),"")</f>
-        <v>1381.8</v>
+        <v>723.80000000000007</v>
       </c>
       <c r="W20" s="56">
         <f>IF($N20&lt;&gt;"",INDEX(Data!$B$9:$J$55,MATCH($N20,Data!$A$9:$A$51,0),MATCH(W$7,Data!$B$4:$AT$4,0)),"")</f>
-        <v>15964.2</v>
+        <v>8362.2000000000007</v>
       </c>
       <c r="X20" s="55">
         <f t="shared" si="7"/>
-        <v>4.3169293241806121E-2</v>
+        <v>4.3169293241806017E-2</v>
       </c>
       <c r="Y20" s="55">
         <f t="shared" si="8"/>
@@ -17999,11 +18000,11 @@
       </c>
       <c r="Z20" s="55">
         <f t="shared" si="9"/>
-        <v>-0.13133077191756903</v>
+        <v>-0.13133077191756909</v>
       </c>
       <c r="AA20" s="55">
         <f t="shared" si="10"/>
-        <v>5.376501611485493E-2</v>
+        <v>5.3765016114854895E-2</v>
       </c>
       <c r="AB20" s="55">
         <f t="shared" si="11"/>
@@ -18011,15 +18012,15 @@
       </c>
       <c r="AC20" s="55">
         <f t="shared" si="12"/>
-        <v>-1.8547750591949509E-2</v>
+        <v>-1.8547750591949529E-2</v>
       </c>
       <c r="AE20" t="str">
         <f t="shared" si="4"/>
-        <v>Pes</v>
+        <v>Minor Liar</v>
       </c>
       <c r="AF20" s="57" cm="1">
         <f t="array" ref="AF20">IF(AE20="","",INDEX(AA20:AC20,$D$6)+(ROW()/10000000000)+N("No row function was used to achieve a unique value to sort"))</f>
-        <v>5.3765018114854929E-2</v>
+        <v>5.3765018114854894E-2</v>
       </c>
       <c r="AG20" s="35"/>
       <c r="AP20" t="s">
@@ -18031,11 +18032,11 @@
       </c>
       <c r="AR20" s="56" cm="1">
         <f t="array" ref="AR20">INDEX(Data!$K$9:$AT$51,MATCH(Calculation!$AP$10,Data!$A$9:$A$51,0),MATCH(Calculation!AR$12&amp;Calculation!$AP20&amp;Calculation!AR$13,INDEX(Data!$K$5:$AT$5&amp;Data!$K$6:$AT$6&amp;Data!$K$7:$AT$7,),0))</f>
-        <v>488</v>
+        <v>459</v>
       </c>
       <c r="AS20" s="56" cm="1">
         <f t="array" ref="AS20">INDEX(Data!$K$9:$AT$51,MATCH(Calculation!$AP$10,Data!$A$9:$A$51,0),MATCH(Calculation!AS$12&amp;Calculation!$AP20&amp;Calculation!AS$13,INDEX(Data!$K$5:$AT$5&amp;Data!$K$6:$AT$6&amp;Data!$K$7:$AT$7,),0))</f>
-        <v>458</v>
+        <v>564</v>
       </c>
       <c r="AU20" t="str">
         <f t="shared" si="15"/>
@@ -18047,11 +18048,11 @@
       </c>
       <c r="AW20" s="85">
         <f t="shared" si="16"/>
-        <v>488</v>
+        <v>459</v>
       </c>
       <c r="AX20" s="85">
         <f t="shared" si="17"/>
-        <v>458</v>
+        <v>564</v>
       </c>
       <c r="AY20" t="e">
         <f t="shared" si="5"/>
@@ -18077,75 +18078,75 @@
       </c>
       <c r="N21" s="46" t="str" cm="1">
         <f t="array" ref="N21">IF(G21&lt;&gt;"",INDEX(G21:I21,,$D$4),"")</f>
-        <v>Baden</v>
+        <v>Mosquit</v>
       </c>
       <c r="O21" s="56">
         <f>IF($N21&lt;&gt;"",INDEX(Data!$B$9:$J$55,MATCH($N21,Data!$A$9:$A$51,0),MATCH(O$7,Data!$B$4:$AT$4,0)),"")</f>
-        <v>35980</v>
+        <v>6302</v>
       </c>
       <c r="P21" s="56">
         <f>IF($N21&lt;&gt;"",INDEX(Data!$B$9:$J$55,MATCH($N21,Data!$A$9:$A$51,0),MATCH(P$7,Data!$B$4:$AT$4,0)),"")</f>
-        <v>2332</v>
+        <v>240</v>
       </c>
       <c r="Q21" s="56">
         <f>IF($N21&lt;&gt;"",INDEX(Data!$B$9:$J$55,MATCH($N21,Data!$A$9:$A$51,0),MATCH(Q$7,Data!$B$4:$AT$4,0)),"")</f>
-        <v>14274</v>
+        <v>4655</v>
       </c>
       <c r="R21" s="56">
         <f>IF($N21&lt;&gt;"",INDEX(Data!$B$9:$J$55,MATCH($N21,Data!$A$9:$A$51,0),MATCH(R$7,Data!$B$4:$AT$4,0)),"")</f>
-        <v>32790</v>
+        <v>5400</v>
       </c>
       <c r="S21" s="56">
         <f>IF($N21&lt;&gt;"",INDEX(Data!$B$9:$J$55,MATCH($N21,Data!$A$9:$A$51,0),MATCH(S$7,Data!$B$4:$AT$4,0)),"")</f>
-        <v>2006</v>
+        <v>190</v>
       </c>
       <c r="T21" s="56">
         <f>IF($N21&lt;&gt;"",INDEX(Data!$B$9:$J$55,MATCH($N21,Data!$A$9:$A$51,0),MATCH(T$7,Data!$B$4:$AT$4,0)),"")</f>
-        <v>14846</v>
+        <v>4096</v>
       </c>
       <c r="U21" s="56">
         <f>IF($N21&lt;&gt;"",INDEX(Data!$B$9:$J$55,MATCH($N21,Data!$A$9:$A$51,0),MATCH(U$7,Data!$B$4:$AT$4,0)),"")</f>
-        <v>36362</v>
+        <v>5293</v>
       </c>
       <c r="V21" s="56">
         <f>IF($N21&lt;&gt;"",INDEX(Data!$B$9:$J$55,MATCH($N21,Data!$A$9:$A$51,0),MATCH(V$7,Data!$B$4:$AT$4,0)),"")</f>
-        <v>2446</v>
+        <v>156</v>
       </c>
       <c r="W21" s="56">
         <f>IF($N21&lt;&gt;"",INDEX(Data!$B$9:$J$55,MATCH($N21,Data!$A$9:$A$51,0),MATCH(W$7,Data!$B$4:$AT$4,0)),"")</f>
-        <v>16392</v>
+        <v>4514</v>
       </c>
       <c r="X21" s="55">
         <f t="shared" si="7"/>
-        <v>9.728575785300396E-2</v>
+        <v>0.16703703703703704</v>
       </c>
       <c r="Y21" s="55">
         <f t="shared" si="8"/>
-        <v>0.16251246261216351</v>
+        <v>0.26315789473684209</v>
       </c>
       <c r="Z21" s="55">
         <f t="shared" si="9"/>
-        <v>-3.8528896672504379E-2</v>
+        <v>0.136474609375</v>
       </c>
       <c r="AA21" s="55">
         <f t="shared" si="10"/>
-        <v>-1.0505472746273583E-2</v>
+        <v>0.19062913281692803</v>
       </c>
       <c r="AB21" s="55">
         <f t="shared" si="11"/>
-        <v>-4.6606704824202781E-2</v>
+        <v>0.53846153846153844</v>
       </c>
       <c r="AC21" s="55">
         <f t="shared" si="12"/>
-        <v>-0.12920937042459738</v>
+        <v>3.1236154186973859E-2</v>
       </c>
       <c r="AE21" t="str">
         <f t="shared" si="4"/>
-        <v>Baden</v>
+        <v>Mosquit</v>
       </c>
       <c r="AF21" s="57" cm="1">
         <f t="array" ref="AF21">IF(AE21="","",INDEX(AA21:AC21,$D$6)+(ROW()/10000000000)+N("No row function was used to achieve a unique value to sort"))</f>
-        <v>-1.0505470646273583E-2</v>
+        <v>0.19062913491692804</v>
       </c>
       <c r="AG21" s="35"/>
       <c r="AI21" s="52"/>
@@ -18158,11 +18159,11 @@
       </c>
       <c r="AR21" s="56" cm="1">
         <f t="array" ref="AR21">INDEX(Data!$K$9:$AT$51,MATCH(Calculation!$AP$10,Data!$A$9:$A$51,0),MATCH(Calculation!AR$12&amp;Calculation!$AP21&amp;Calculation!AR$13,INDEX(Data!$K$5:$AT$5&amp;Data!$K$6:$AT$6&amp;Data!$K$7:$AT$7,),0))</f>
-        <v>464</v>
+        <v>536</v>
       </c>
       <c r="AS21" s="56" cm="1">
         <f t="array" ref="AS21">INDEX(Data!$K$9:$AT$51,MATCH(Calculation!$AP$10,Data!$A$9:$A$51,0),MATCH(Calculation!AS$12&amp;Calculation!$AP21&amp;Calculation!AS$13,INDEX(Data!$K$5:$AT$5&amp;Data!$K$6:$AT$6&amp;Data!$K$7:$AT$7,),0))</f>
-        <v>453</v>
+        <v>645</v>
       </c>
       <c r="AU21" t="str">
         <f t="shared" si="15"/>
@@ -18174,11 +18175,11 @@
       </c>
       <c r="AW21" s="85">
         <f t="shared" si="16"/>
-        <v>464</v>
+        <v>536</v>
       </c>
       <c r="AX21" s="85">
         <f t="shared" si="17"/>
-        <v>453</v>
+        <v>645</v>
       </c>
       <c r="AY21" t="e">
         <f t="shared" si="5"/>
@@ -18204,75 +18205,75 @@
       </c>
       <c r="N22" s="46" t="str" cm="1">
         <f t="array" ref="N22">IF(G22&lt;&gt;"",INDEX(G22:I22,,$D$4),"")</f>
-        <v>Jellyfish</v>
+        <v>Atmos</v>
       </c>
       <c r="O22" s="56">
         <f>IF($N22&lt;&gt;"",INDEX(Data!$B$9:$J$55,MATCH($N22,Data!$A$9:$A$51,0),MATCH(O$7,Data!$B$4:$AT$4,0)),"")</f>
-        <v>7657</v>
+        <v>10675</v>
       </c>
       <c r="P22" s="56">
         <f>IF($N22&lt;&gt;"",INDEX(Data!$B$9:$J$55,MATCH($N22,Data!$A$9:$A$51,0),MATCH(P$7,Data!$B$4:$AT$4,0)),"")</f>
-        <v>276</v>
+        <v>128</v>
       </c>
       <c r="Q22" s="56">
         <f>IF($N22&lt;&gt;"",INDEX(Data!$B$9:$J$55,MATCH($N22,Data!$A$9:$A$51,0),MATCH(Q$7,Data!$B$4:$AT$4,0)),"")</f>
-        <v>5353</v>
+        <v>8210</v>
       </c>
       <c r="R22" s="56">
         <f>IF($N22&lt;&gt;"",INDEX(Data!$B$9:$J$55,MATCH($N22,Data!$A$9:$A$51,0),MATCH(R$7,Data!$B$4:$AT$4,0)),"")</f>
-        <v>5307</v>
+        <v>10133</v>
       </c>
       <c r="S22" s="56">
         <f>IF($N22&lt;&gt;"",INDEX(Data!$B$9:$J$55,MATCH($N22,Data!$A$9:$A$51,0),MATCH(S$7,Data!$B$4:$AT$4,0)),"")</f>
-        <v>170</v>
+        <v>89</v>
       </c>
       <c r="T22" s="56">
         <f>IF($N22&lt;&gt;"",INDEX(Data!$B$9:$J$55,MATCH($N22,Data!$A$9:$A$51,0),MATCH(T$7,Data!$B$4:$AT$4,0)),"")</f>
-        <v>4710</v>
+        <v>8179</v>
       </c>
       <c r="U22" s="56">
         <f>IF($N22&lt;&gt;"",INDEX(Data!$B$9:$J$55,MATCH($N22,Data!$A$9:$A$51,0),MATCH(U$7,Data!$B$4:$AT$4,0)),"")</f>
-        <v>6431</v>
+        <v>11178</v>
       </c>
       <c r="V22" s="56">
         <f>IF($N22&lt;&gt;"",INDEX(Data!$B$9:$J$55,MATCH($N22,Data!$A$9:$A$51,0),MATCH(V$7,Data!$B$4:$AT$4,0)),"")</f>
-        <v>179</v>
+        <v>190</v>
       </c>
       <c r="W22" s="56">
         <f>IF($N22&lt;&gt;"",INDEX(Data!$B$9:$J$55,MATCH($N22,Data!$A$9:$A$51,0),MATCH(W$7,Data!$B$4:$AT$4,0)),"")</f>
-        <v>5191</v>
+        <v>8010</v>
       </c>
       <c r="X22" s="55">
         <f t="shared" si="7"/>
-        <v>0.44281138119464858</v>
+        <v>5.34886015987368E-2</v>
       </c>
       <c r="Y22" s="55">
         <f t="shared" si="8"/>
-        <v>0.62352941176470589</v>
+        <v>0.43820224719101125</v>
       </c>
       <c r="Z22" s="55">
         <f t="shared" si="9"/>
-        <v>0.13651804670912951</v>
+        <v>3.7901944002934345E-3</v>
       </c>
       <c r="AA22" s="55">
         <f t="shared" si="10"/>
-        <v>0.19063909189861608</v>
+        <v>-4.4999105385578816E-2</v>
       </c>
       <c r="AB22" s="55">
         <f t="shared" si="11"/>
-        <v>0.54189944134078216</v>
+        <v>-0.32631578947368423</v>
       </c>
       <c r="AC22" s="55">
         <f t="shared" si="12"/>
-        <v>3.1207859757272201E-2</v>
+        <v>2.4968789013732832E-2</v>
       </c>
       <c r="AE22" t="str">
         <f t="shared" si="4"/>
-        <v>Jellyfish</v>
+        <v>Atmos</v>
       </c>
       <c r="AF22" s="57" cm="1">
         <f t="array" ref="AF22">IF(AE22="","",INDEX(AA22:AC22,$D$6)+(ROW()/10000000000)+N("No row function was used to achieve a unique value to sort"))</f>
-        <v>0.19063909409861607</v>
+        <v>-4.4999103185578815E-2</v>
       </c>
       <c r="AG22" s="35"/>
       <c r="AP22" t="s">
@@ -18284,11 +18285,11 @@
       </c>
       <c r="AR22" s="56" cm="1">
         <f t="array" ref="AR22">INDEX(Data!$K$9:$AT$51,MATCH(Calculation!$AP$10,Data!$A$9:$A$51,0),MATCH(Calculation!AR$12&amp;Calculation!$AP22&amp;Calculation!AR$13,INDEX(Data!$K$5:$AT$5&amp;Data!$K$6:$AT$6&amp;Data!$K$7:$AT$7,),0))</f>
-        <v>429</v>
+        <v>629</v>
       </c>
       <c r="AS22" s="56" cm="1">
         <f t="array" ref="AS22">INDEX(Data!$K$9:$AT$51,MATCH(Calculation!$AP$10,Data!$A$9:$A$51,0),MATCH(Calculation!AS$12&amp;Calculation!$AP22&amp;Calculation!AS$13,INDEX(Data!$K$5:$AT$5&amp;Data!$K$6:$AT$6&amp;Data!$K$7:$AT$7,),0))</f>
-        <v>522</v>
+        <v>688</v>
       </c>
       <c r="AU22" t="str">
         <f t="shared" si="15"/>
@@ -18300,15 +18301,15 @@
       </c>
       <c r="AW22" s="85">
         <f t="shared" si="16"/>
-        <v>429</v>
+        <v>629</v>
       </c>
       <c r="AX22" s="85">
         <f t="shared" si="17"/>
-        <v>522</v>
-      </c>
-      <c r="AY22">
+        <v>688</v>
+      </c>
+      <c r="AY22" t="e">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="23" spans="2:51" x14ac:dyDescent="0.25">
@@ -18330,75 +18331,75 @@
       </c>
       <c r="N23" s="46" t="str" cm="1">
         <f t="array" ref="N23">IF(G23&lt;&gt;"",INDEX(G23:I23,,$D$4),"")</f>
-        <v>Aviatrr</v>
+        <v>Scrap</v>
       </c>
       <c r="O23" s="56">
         <f>IF($N23&lt;&gt;"",INDEX(Data!$B$9:$J$55,MATCH($N23,Data!$A$9:$A$51,0),MATCH(O$7,Data!$B$4:$AT$4,0)),"")</f>
-        <v>8126</v>
+        <v>13307</v>
       </c>
       <c r="P23" s="56">
         <f>IF($N23&lt;&gt;"",INDEX(Data!$B$9:$J$55,MATCH($N23,Data!$A$9:$A$51,0),MATCH(P$7,Data!$B$4:$AT$4,0)),"")</f>
-        <v>321</v>
+        <v>862</v>
       </c>
       <c r="Q23" s="56">
         <f>IF($N23&lt;&gt;"",INDEX(Data!$B$9:$J$55,MATCH($N23,Data!$A$9:$A$51,0),MATCH(Q$7,Data!$B$4:$AT$4,0)),"")</f>
-        <v>6153</v>
+        <v>5279</v>
       </c>
       <c r="R23" s="56">
         <f>IF($N23&lt;&gt;"",INDEX(Data!$B$9:$J$55,MATCH($N23,Data!$A$9:$A$51,0),MATCH(R$7,Data!$B$4:$AT$4,0)),"")</f>
-        <v>9111</v>
+        <v>12127</v>
       </c>
       <c r="S23" s="56">
         <f>IF($N23&lt;&gt;"",INDEX(Data!$B$9:$J$55,MATCH($N23,Data!$A$9:$A$51,0),MATCH(S$7,Data!$B$4:$AT$4,0)),"")</f>
-        <v>567</v>
+        <v>742</v>
       </c>
       <c r="T23" s="56">
         <f>IF($N23&lt;&gt;"",INDEX(Data!$B$9:$J$55,MATCH($N23,Data!$A$9:$A$51,0),MATCH(T$7,Data!$B$4:$AT$4,0)),"")</f>
-        <v>5959</v>
+        <v>5491</v>
       </c>
       <c r="U23" s="56">
         <f>IF($N23&lt;&gt;"",INDEX(Data!$B$9:$J$55,MATCH($N23,Data!$A$9:$A$51,0),MATCH(U$7,Data!$B$4:$AT$4,0)),"")</f>
-        <v>8642</v>
+        <v>13448</v>
       </c>
       <c r="V23" s="56">
         <f>IF($N23&lt;&gt;"",INDEX(Data!$B$9:$J$55,MATCH($N23,Data!$A$9:$A$51,0),MATCH(V$7,Data!$B$4:$AT$4,0)),"")</f>
-        <v>554</v>
+        <v>905</v>
       </c>
       <c r="W23" s="56">
         <f>IF($N23&lt;&gt;"",INDEX(Data!$B$9:$J$55,MATCH($N23,Data!$A$9:$A$51,0),MATCH(W$7,Data!$B$4:$AT$4,0)),"")</f>
-        <v>7382</v>
+        <v>6062</v>
       </c>
       <c r="X23" s="55">
         <f t="shared" si="7"/>
-        <v>-0.10811107452529908</v>
+        <v>9.730353756081471E-2</v>
       </c>
       <c r="Y23" s="55">
         <f t="shared" si="8"/>
-        <v>-0.43386243386243384</v>
+        <v>0.16172506738544473</v>
       </c>
       <c r="Z23" s="55">
         <f t="shared" si="9"/>
-        <v>3.2555797952676623E-2</v>
+        <v>-3.8608632307412127E-2</v>
       </c>
       <c r="AA23" s="55">
         <f t="shared" si="10"/>
-        <v>-5.9708400833140475E-2</v>
+        <v>-1.0484830458060678E-2</v>
       </c>
       <c r="AB23" s="55">
         <f t="shared" si="11"/>
-        <v>-0.42057761732851984</v>
+        <v>-4.7513812154696133E-2</v>
       </c>
       <c r="AC23" s="55">
         <f t="shared" si="12"/>
-        <v>-0.16648604714169601</v>
+        <v>-0.12916529198284393</v>
       </c>
       <c r="AE23" t="str">
         <f t="shared" si="4"/>
-        <v>Aviatrr</v>
+        <v>Scrap</v>
       </c>
       <c r="AF23" s="57" cm="1">
         <f t="array" ref="AF23">IF(AE23="","",INDEX(AA23:AC23,$D$6)+(ROW()/10000000000)+N("No row function was used to achieve a unique value to sort"))</f>
-        <v>-5.9708398533140472E-2</v>
+        <v>-1.0484828158060679E-2</v>
       </c>
       <c r="AG23" s="35"/>
       <c r="AI23" s="73"/>
@@ -18412,27 +18413,27 @@
       </c>
       <c r="AR23" s="56" cm="1">
         <f t="array" ref="AR23">INDEX(Data!$K$9:$AT$51,MATCH(Calculation!$AP$10,Data!$A$9:$A$51,0),MATCH(Calculation!AR$12&amp;Calculation!$AP23&amp;Calculation!AR$13,INDEX(Data!$K$5:$AT$5&amp;Data!$K$6:$AT$6&amp;Data!$K$7:$AT$7,),0))</f>
-        <v>430</v>
+        <v>656</v>
       </c>
       <c r="AS23" s="56" cm="1">
         <f t="array" ref="AS23">INDEX(Data!$K$9:$AT$51,MATCH(Calculation!$AP$10,Data!$A$9:$A$51,0),MATCH(Calculation!AS$12&amp;Calculation!$AP23&amp;Calculation!AS$13,INDEX(Data!$K$5:$AT$5&amp;Data!$K$6:$AT$6&amp;Data!$K$7:$AT$7,),0))</f>
-        <v>566</v>
+        <v>706</v>
       </c>
       <c r="AU23" t="str">
         <f t="shared" si="15"/>
         <v>O</v>
       </c>
-      <c r="AV23" t="e">
+      <c r="AV23">
         <f>IF(MATCH(cur_month,$AP$14:$AP$25,0)&gt;=ROWS(AP$14:$AP23),AQ23,NA())</f>
-        <v>#N/A</v>
+        <v>0</v>
       </c>
       <c r="AW23" s="85">
         <f t="shared" si="16"/>
-        <v>430</v>
+        <v>656</v>
       </c>
       <c r="AX23" s="85">
         <f t="shared" si="17"/>
-        <v>566</v>
+        <v>706</v>
       </c>
       <c r="AY23" t="e">
         <f t="shared" si="5"/>
@@ -18458,75 +18459,75 @@
       </c>
       <c r="N24" s="46" t="str" cm="1">
         <f t="array" ref="N24">IF(G24&lt;&gt;"",INDEX(G24:I24,,$D$4),"")</f>
-        <v>deRamblr</v>
+        <v>Motocyco</v>
       </c>
       <c r="O24" s="56">
         <f>IF($N24&lt;&gt;"",INDEX(Data!$B$9:$J$55,MATCH($N24,Data!$A$9:$A$51,0),MATCH(O$7,Data!$B$4:$AT$4,0)),"")</f>
-        <v>5272</v>
+        <v>11182</v>
       </c>
       <c r="P24" s="56">
         <f>IF($N24&lt;&gt;"",INDEX(Data!$B$9:$J$55,MATCH($N24,Data!$A$9:$A$51,0),MATCH(P$7,Data!$B$4:$AT$4,0)),"")</f>
-        <v>316</v>
+        <v>1193</v>
       </c>
       <c r="Q24" s="56">
         <f>IF($N24&lt;&gt;"",INDEX(Data!$B$9:$J$55,MATCH($N24,Data!$A$9:$A$51,0),MATCH(Q$7,Data!$B$4:$AT$4,0)),"")</f>
-        <v>1207</v>
+        <v>4311</v>
       </c>
       <c r="R24" s="56">
         <f>IF($N24&lt;&gt;"",INDEX(Data!$B$9:$J$55,MATCH($N24,Data!$A$9:$A$51,0),MATCH(R$7,Data!$B$4:$AT$4,0)),"")</f>
-        <v>4934</v>
+        <v>10457</v>
       </c>
       <c r="S24" s="56">
         <f>IF($N24&lt;&gt;"",INDEX(Data!$B$9:$J$55,MATCH($N24,Data!$A$9:$A$51,0),MATCH(S$7,Data!$B$4:$AT$4,0)),"")</f>
-        <v>233</v>
+        <v>890</v>
       </c>
       <c r="T24" s="56">
         <f>IF($N24&lt;&gt;"",INDEX(Data!$B$9:$J$55,MATCH($N24,Data!$A$9:$A$51,0),MATCH(T$7,Data!$B$4:$AT$4,0)),"")</f>
-        <v>1485</v>
+        <v>4595</v>
       </c>
       <c r="U24" s="56">
         <f>IF($N24&lt;&gt;"",INDEX(Data!$B$9:$J$55,MATCH($N24,Data!$A$9:$A$51,0),MATCH(U$7,Data!$B$4:$AT$4,0)),"")</f>
-        <v>4789</v>
+        <v>9952</v>
       </c>
       <c r="V24" s="56">
         <f>IF($N24&lt;&gt;"",INDEX(Data!$B$9:$J$55,MATCH($N24,Data!$A$9:$A$51,0),MATCH(V$7,Data!$B$4:$AT$4,0)),"")</f>
-        <v>215</v>
+        <v>810</v>
       </c>
       <c r="W24" s="56">
         <f>IF($N24&lt;&gt;"",INDEX(Data!$B$9:$J$55,MATCH($N24,Data!$A$9:$A$51,0),MATCH(W$7,Data!$B$4:$AT$4,0)),"")</f>
-        <v>1936</v>
+        <v>4298</v>
       </c>
       <c r="X24" s="55">
         <f t="shared" si="7"/>
-        <v>6.8504256181597084E-2</v>
+        <v>6.9331548245194607E-2</v>
       </c>
       <c r="Y24" s="55">
         <f t="shared" si="8"/>
-        <v>0.35622317596566522</v>
+        <v>0.34044943820224721</v>
       </c>
       <c r="Z24" s="55">
         <f t="shared" si="9"/>
-        <v>-0.18720538720538721</v>
+        <v>-6.1806311207834599E-2</v>
       </c>
       <c r="AA24" s="55">
         <f t="shared" si="10"/>
-        <v>0.10085612862810607</v>
+        <v>0.12359324758842444</v>
       </c>
       <c r="AB24" s="55">
         <f t="shared" si="11"/>
-        <v>0.4697674418604651</v>
+        <v>0.47283950617283949</v>
       </c>
       <c r="AC24" s="55">
         <f t="shared" si="12"/>
-        <v>-0.37654958677685951</v>
+        <v>3.0246626337831549E-3</v>
       </c>
       <c r="AE24" t="str">
         <f t="shared" si="4"/>
-        <v>deRamblr</v>
+        <v>Motocyco</v>
       </c>
       <c r="AF24" s="57" cm="1">
         <f t="array" ref="AF24">IF(AE24="","",INDEX(AA24:AC24,$D$6)+(ROW()/10000000000)+N("No row function was used to achieve a unique value to sort"))</f>
-        <v>0.10085613102810607</v>
+        <v>0.12359324998842444</v>
       </c>
       <c r="AG24" s="35"/>
       <c r="AI24" s="73"/>
@@ -18540,27 +18541,27 @@
       </c>
       <c r="AR24" s="56" cm="1">
         <f t="array" ref="AR24">INDEX(Data!$K$9:$AT$51,MATCH(Calculation!$AP$10,Data!$A$9:$A$51,0),MATCH(Calculation!AR$12&amp;Calculation!$AP24&amp;Calculation!AR$13,INDEX(Data!$K$5:$AT$5&amp;Data!$K$6:$AT$6&amp;Data!$K$7:$AT$7,),0))</f>
-        <v>432</v>
+        <v>641</v>
       </c>
       <c r="AS24" s="56" cm="1">
         <f t="array" ref="AS24">INDEX(Data!$K$9:$AT$51,MATCH(Calculation!$AP$10,Data!$A$9:$A$51,0),MATCH(Calculation!AS$12&amp;Calculation!$AP24&amp;Calculation!AS$13,INDEX(Data!$K$5:$AT$5&amp;Data!$K$6:$AT$6&amp;Data!$K$7:$AT$7,),0))</f>
-        <v>596</v>
+        <v>664</v>
       </c>
       <c r="AU24" t="str">
         <f t="shared" si="15"/>
         <v>N</v>
       </c>
-      <c r="AV24" t="e">
+      <c r="AV24">
         <f>IF(MATCH(cur_month,$AP$14:$AP$25,0)&gt;=ROWS(AP$14:$AP24),AQ24,NA())</f>
-        <v>#N/A</v>
+        <v>0</v>
       </c>
       <c r="AW24" s="85">
         <f t="shared" si="16"/>
-        <v>432</v>
+        <v>641</v>
       </c>
       <c r="AX24" s="85">
         <f t="shared" si="17"/>
-        <v>596</v>
+        <v>664</v>
       </c>
       <c r="AY24" t="e">
         <f t="shared" si="5"/>
@@ -18586,75 +18587,75 @@
       </c>
       <c r="N25" s="46" t="str" cm="1">
         <f t="array" ref="N25">IF(G25&lt;&gt;"",INDEX(G25:I25,,$D$4),"")</f>
-        <v>Arcade</v>
+        <v>Amplefio</v>
       </c>
       <c r="O25" s="56">
         <f>IF($N25&lt;&gt;"",INDEX(Data!$B$9:$J$55,MATCH($N25,Data!$A$9:$A$51,0),MATCH(O$7,Data!$B$4:$AT$4,0)),"")</f>
-        <v>6375</v>
+        <v>8250</v>
       </c>
       <c r="P25" s="56">
         <f>IF($N25&lt;&gt;"",INDEX(Data!$B$9:$J$55,MATCH($N25,Data!$A$9:$A$51,0),MATCH(P$7,Data!$B$4:$AT$4,0)),"")</f>
-        <v>192</v>
+        <v>541</v>
       </c>
       <c r="Q25" s="56">
         <f>IF($N25&lt;&gt;"",INDEX(Data!$B$9:$J$55,MATCH($N25,Data!$A$9:$A$51,0),MATCH(Q$7,Data!$B$4:$AT$4,0)),"")</f>
-        <v>4741</v>
+        <v>5923</v>
       </c>
       <c r="R25" s="56">
         <f>IF($N25&lt;&gt;"",INDEX(Data!$B$9:$J$55,MATCH($N25,Data!$A$9:$A$51,0),MATCH(R$7,Data!$B$4:$AT$4,0)),"")</f>
-        <v>6945</v>
+        <v>8507</v>
       </c>
       <c r="S25" s="56">
         <f>IF($N25&lt;&gt;"",INDEX(Data!$B$9:$J$55,MATCH($N25,Data!$A$9:$A$51,0),MATCH(S$7,Data!$B$4:$AT$4,0)),"")</f>
-        <v>309</v>
+        <v>369</v>
       </c>
       <c r="T25" s="56">
         <f>IF($N25&lt;&gt;"",INDEX(Data!$B$9:$J$55,MATCH($N25,Data!$A$9:$A$51,0),MATCH(T$7,Data!$B$4:$AT$4,0)),"")</f>
-        <v>5006</v>
+        <v>6622</v>
       </c>
       <c r="U25" s="56">
         <f>IF($N25&lt;&gt;"",INDEX(Data!$B$9:$J$55,MATCH($N25,Data!$A$9:$A$51,0),MATCH(U$7,Data!$B$4:$AT$4,0)),"")</f>
-        <v>5774</v>
+        <v>8899</v>
       </c>
       <c r="V25" s="56">
         <f>IF($N25&lt;&gt;"",INDEX(Data!$B$9:$J$55,MATCH($N25,Data!$A$9:$A$51,0),MATCH(V$7,Data!$B$4:$AT$4,0)),"")</f>
-        <v>350</v>
+        <v>474</v>
       </c>
       <c r="W25" s="56">
         <f>IF($N25&lt;&gt;"",INDEX(Data!$B$9:$J$55,MATCH($N25,Data!$A$9:$A$51,0),MATCH(W$7,Data!$B$4:$AT$4,0)),"")</f>
-        <v>4447</v>
+        <v>6231</v>
       </c>
       <c r="X25" s="55">
         <f t="shared" si="7"/>
-        <v>-8.2073434125269976E-2</v>
+        <v>-3.0210414952392149E-2</v>
       </c>
       <c r="Y25" s="55">
         <f t="shared" si="8"/>
-        <v>-0.37864077669902912</v>
+        <v>0.46612466124661245</v>
       </c>
       <c r="Z25" s="55">
         <f t="shared" si="9"/>
-        <v>-5.2936476228525771E-2</v>
+        <v>-0.10555723346421021</v>
       </c>
       <c r="AA25" s="55">
         <f t="shared" si="10"/>
-        <v>0.10408728784205057</v>
+        <v>-7.2929542645241041E-2</v>
       </c>
       <c r="AB25" s="55">
         <f t="shared" si="11"/>
-        <v>-0.4514285714285714</v>
+        <v>0.14135021097046413</v>
       </c>
       <c r="AC25" s="55">
         <f t="shared" si="12"/>
-        <v>6.6111985608275248E-2</v>
+        <v>-4.9430268014764883E-2</v>
       </c>
       <c r="AE25" t="str">
         <f t="shared" si="4"/>
-        <v>Arcade</v>
+        <v>Amplefio</v>
       </c>
       <c r="AF25" s="57" cm="1">
         <f t="array" ref="AF25">IF(AE25="","",INDEX(AA25:AC25,$D$6)+(ROW()/10000000000)+N("No row function was used to achieve a unique value to sort"))</f>
-        <v>0.10408729034205057</v>
+        <v>-7.2929540145241042E-2</v>
       </c>
       <c r="AG25" s="35"/>
       <c r="AI25" s="73"/>
@@ -18668,31 +18669,31 @@
       </c>
       <c r="AR25" s="56" cm="1">
         <f t="array" ref="AR25">INDEX(Data!$K$9:$AT$51,MATCH(Calculation!$AP$10,Data!$A$9:$A$51,0),MATCH(Calculation!AR$12&amp;Calculation!$AP25&amp;Calculation!AR$13,INDEX(Data!$K$5:$AT$5&amp;Data!$K$6:$AT$6&amp;Data!$K$7:$AT$7,),0))</f>
-        <v>435</v>
+        <v>550</v>
       </c>
       <c r="AS25" s="56" cm="1">
         <f t="array" ref="AS25">INDEX(Data!$K$9:$AT$51,MATCH(Calculation!$AP$10,Data!$A$9:$A$51,0),MATCH(Calculation!AS$12&amp;Calculation!$AP25&amp;Calculation!AS$13,INDEX(Data!$K$5:$AT$5&amp;Data!$K$6:$AT$6&amp;Data!$K$7:$AT$7,),0))</f>
-        <v>591</v>
+        <v>593</v>
       </c>
       <c r="AU25" t="str">
         <f t="shared" si="15"/>
         <v>D</v>
       </c>
-      <c r="AV25" t="e">
+      <c r="AV25">
         <f>IF(MATCH(cur_month,$AP$14:$AP$25,0)&gt;=ROWS(AP$14:$AP25),AQ25,NA())</f>
-        <v>#N/A</v>
+        <v>0</v>
       </c>
       <c r="AW25" s="85">
         <f t="shared" si="16"/>
-        <v>435</v>
+        <v>550</v>
       </c>
       <c r="AX25" s="85">
         <f t="shared" si="17"/>
-        <v>591</v>
-      </c>
-      <c r="AY25" t="e">
+        <v>593</v>
+      </c>
+      <c r="AY25">
         <f t="shared" si="5"/>
-        <v>#N/A</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="2:51" x14ac:dyDescent="0.25">
@@ -18705,81 +18706,81 @@
       <c r="I26" s="42" t="s">
         <v>74</v>
       </c>
-      <c r="M26" s="37" t="str">
+      <c r="M26" s="37">
         <f t="shared" si="6"/>
-        <v/>
+        <v>13</v>
       </c>
       <c r="N26" s="46" t="str" cm="1">
         <f t="array" ref="N26">IF(G26&lt;&gt;"",INDEX(G26:I26,,$D$4),"")</f>
-        <v/>
-      </c>
-      <c r="O26" s="56" t="str">
+        <v>Strex</v>
+      </c>
+      <c r="O26" s="56">
         <f>IF($N26&lt;&gt;"",INDEX(Data!$B$9:$J$55,MATCH($N26,Data!$A$9:$A$51,0),MATCH(O$7,Data!$B$4:$AT$4,0)),"")</f>
-        <v/>
-      </c>
-      <c r="P26" s="56" t="str">
+        <v>8152</v>
+      </c>
+      <c r="P26" s="56">
         <f>IF($N26&lt;&gt;"",INDEX(Data!$B$9:$J$55,MATCH($N26,Data!$A$9:$A$51,0),MATCH(P$7,Data!$B$4:$AT$4,0)),"")</f>
-        <v/>
-      </c>
-      <c r="Q26" s="56" t="str">
+        <v>258</v>
+      </c>
+      <c r="Q26" s="56">
         <f>IF($N26&lt;&gt;"",INDEX(Data!$B$9:$J$55,MATCH($N26,Data!$A$9:$A$51,0),MATCH(Q$7,Data!$B$4:$AT$4,0)),"")</f>
-        <v/>
-      </c>
-      <c r="R26" s="56" t="str">
+        <v>5700</v>
+      </c>
+      <c r="R26" s="56">
         <f>IF($N26&lt;&gt;"",INDEX(Data!$B$9:$J$55,MATCH($N26,Data!$A$9:$A$51,0),MATCH(R$7,Data!$B$4:$AT$4,0)),"")</f>
-        <v/>
-      </c>
-      <c r="S26" s="56" t="str">
+        <v>10832</v>
+      </c>
+      <c r="S26" s="56">
         <f>IF($N26&lt;&gt;"",INDEX(Data!$B$9:$J$55,MATCH($N26,Data!$A$9:$A$51,0),MATCH(S$7,Data!$B$4:$AT$4,0)),"")</f>
-        <v/>
-      </c>
-      <c r="T26" s="56" t="str">
+        <v>577</v>
+      </c>
+      <c r="T26" s="56">
         <f>IF($N26&lt;&gt;"",INDEX(Data!$B$9:$J$55,MATCH($N26,Data!$A$9:$A$51,0),MATCH(T$7,Data!$B$4:$AT$4,0)),"")</f>
-        <v/>
-      </c>
-      <c r="U26" s="56" t="str">
+        <v>5100</v>
+      </c>
+      <c r="U26" s="56">
         <f>IF($N26&lt;&gt;"",INDEX(Data!$B$9:$J$55,MATCH($N26,Data!$A$9:$A$51,0),MATCH(U$7,Data!$B$4:$AT$4,0)),"")</f>
-        <v/>
-      </c>
-      <c r="V26" s="56" t="str">
+        <v>9698</v>
+      </c>
+      <c r="V26" s="56">
         <f>IF($N26&lt;&gt;"",INDEX(Data!$B$9:$J$55,MATCH($N26,Data!$A$9:$A$51,0),MATCH(V$7,Data!$B$4:$AT$4,0)),"")</f>
-        <v/>
-      </c>
-      <c r="W26" s="56" t="str">
+        <v>350</v>
+      </c>
+      <c r="W26" s="56">
         <f>IF($N26&lt;&gt;"",INDEX(Data!$B$9:$J$55,MATCH($N26,Data!$A$9:$A$51,0),MATCH(W$7,Data!$B$4:$AT$4,0)),"")</f>
-        <v/>
-      </c>
-      <c r="X26" s="55" t="str">
+        <v>5200</v>
+      </c>
+      <c r="X26" s="55">
         <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="Y26" s="55" t="str">
+        <v>-0.24741506646971936</v>
+      </c>
+      <c r="Y26" s="55">
         <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="Z26" s="55" t="str">
+        <v>-0.55285961871750433</v>
+      </c>
+      <c r="Z26" s="55">
         <f t="shared" si="9"/>
-        <v/>
-      </c>
-      <c r="AA26" s="55" t="str">
+        <v>0.11764705882352941</v>
+      </c>
+      <c r="AA26" s="55">
         <f t="shared" si="10"/>
-        <v/>
-      </c>
-      <c r="AB26" s="55" t="str">
+        <v>-0.15941431222932564</v>
+      </c>
+      <c r="AB26" s="55">
         <f t="shared" si="11"/>
-        <v/>
-      </c>
-      <c r="AC26" s="55" t="str">
+        <v>-0.26285714285714284</v>
+      </c>
+      <c r="AC26" s="55">
         <f t="shared" si="12"/>
-        <v/>
+        <v>9.6153846153846159E-2</v>
       </c>
       <c r="AE26" t="str">
         <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="AF26" s="57" t="str" cm="1">
+        <v>Strex</v>
+      </c>
+      <c r="AF26" s="57" cm="1">
         <f t="array" ref="AF26">IF(AE26="","",INDEX(AA26:AC26,$D$6)+(ROW()/10000000000)+N("No row function was used to achieve a unique value to sort"))</f>
-        <v/>
+        <v>-0.15941430962932565</v>
       </c>
       <c r="AG26" s="35"/>
       <c r="AI26" s="73"/>
@@ -19477,67 +19478,67 @@
     <row r="36" spans="7:33" x14ac:dyDescent="0.25">
       <c r="N36" s="46" t="str" cm="1">
         <f t="array" ref="N36">INDEX($G$13:$I$13,$D$4)</f>
-        <v>Game Apps</v>
+        <v>Utility Apps</v>
       </c>
       <c r="O36" s="65">
         <f>IF($N36&lt;&gt;"",INDEX(Data!$B$9:$J$55,MATCH($N36,Data!$A$9:$A$51,0),MATCH(O$7,Data!$B$4:$AT$4,0)),"")</f>
-        <v>210616</v>
+        <v>189978.5</v>
       </c>
       <c r="P36" s="65">
         <f>IF($N36&lt;&gt;"",INDEX(Data!$B$9:$J$55,MATCH($N36,Data!$A$9:$A$51,0),MATCH(P$7,Data!$B$4:$AT$4,0)),"")</f>
-        <v>12324.3</v>
+        <v>8869.2000000000007</v>
       </c>
       <c r="Q36" s="65">
         <f>IF($N36&lt;&gt;"",INDEX(Data!$B$9:$J$55,MATCH($N36,Data!$A$9:$A$51,0),MATCH(Q$7,Data!$B$4:$AT$4,0)),"")</f>
-        <v>95902.1</v>
+        <v>91467.1</v>
       </c>
       <c r="R36" s="65">
         <f>IF($N36&lt;&gt;"",INDEX(Data!$B$9:$J$55,MATCH($N36,Data!$A$9:$A$51,0),MATCH(R$7,Data!$B$4:$AT$4,0)),"")</f>
-        <v>199893.6</v>
+        <v>187118.2</v>
       </c>
       <c r="S36" s="65">
         <f>IF($N36&lt;&gt;"",INDEX(Data!$B$9:$J$55,MATCH($N36,Data!$A$9:$A$51,0),MATCH(S$7,Data!$B$4:$AT$4,0)),"")</f>
-        <v>9835.9000000000015</v>
+        <v>7865.9000000000005</v>
       </c>
       <c r="T36" s="65">
         <f>IF($N36&lt;&gt;"",INDEX(Data!$B$9:$J$55,MATCH($N36,Data!$A$9:$A$51,0),MATCH(T$7,Data!$B$4:$AT$4,0)),"")</f>
-        <v>101383.6</v>
+        <v>97100.299999999988</v>
       </c>
       <c r="U36" s="65">
         <f>IF($N36&lt;&gt;"",INDEX(Data!$B$9:$J$55,MATCH($N36,Data!$A$9:$A$51,0),MATCH(U$7,Data!$B$4:$AT$4,0)),"")</f>
-        <v>198526.40000000002</v>
+        <v>181464.8</v>
       </c>
       <c r="V36" s="65">
         <f>IF($N36&lt;&gt;"",INDEX(Data!$B$9:$J$55,MATCH($N36,Data!$A$9:$A$51,0),MATCH(V$7,Data!$B$4:$AT$4,0)),"")</f>
-        <v>11343.8</v>
+        <v>8122.2</v>
       </c>
       <c r="W36" s="65">
         <f>IF($N36&lt;&gt;"",INDEX(Data!$B$9:$J$55,MATCH($N36,Data!$A$9:$A$51,0),MATCH(W$7,Data!$B$4:$AT$4,0)),"")</f>
-        <v>100022.6</v>
+        <v>94780.800000000003</v>
       </c>
       <c r="X36" s="53">
         <f t="shared" ref="X36" si="23">IF($N36&lt;&gt;"",(O36-R36)/R36,"")</f>
-        <v>5.3640536765559244E-2</v>
+        <v>1.5286059827424528E-2</v>
       </c>
       <c r="Y36" s="53">
         <f t="shared" ref="Y36" si="24">IF($N36&lt;&gt;"",(P36-S36)/S36,"")</f>
-        <v>0.25299159202513216</v>
+        <v>0.12755056636875628</v>
       </c>
       <c r="Z36" s="53">
         <f t="shared" ref="Z36" si="25">IF($N36&lt;&gt;"",(Q36-T36)/T36,"")</f>
-        <v>-5.4066929957113374E-2</v>
+        <v>-5.8014238884946633E-2</v>
       </c>
       <c r="AA36" s="53">
         <f t="shared" ref="AA36" si="26">IF($N36&lt;&gt;"",(O36-U36)/U36,"")</f>
-        <v>6.0896686788255744E-2</v>
+        <v>4.6916536981276874E-2</v>
       </c>
       <c r="AB36" s="53">
         <f t="shared" ref="AB36" si="27">IF($N36&lt;&gt;"",(P36-V36)/V36,"")</f>
-        <v>8.6434880727798452E-2</v>
+        <v>9.1970155869099623E-2</v>
       </c>
       <c r="AC36" s="53">
         <f t="shared" ref="AC36" si="28">IF($N36&lt;&gt;"",(Q36-W36)/W36,"")</f>
-        <v>-4.1195689774111047E-2</v>
+        <v>-3.4961722205341134E-2</v>
       </c>
     </row>
     <row r="38" spans="7:33" x14ac:dyDescent="0.25">
@@ -19566,7 +19567,7 @@
       </c>
       <c r="O39" s="66">
         <f>O36-U36</f>
-        <v>12089.599999999977</v>
+        <v>8513.7000000000116</v>
       </c>
       <c r="P39" t="str">
         <f>IF(O39&gt;0,"Over Budget","Under Budget")</f>
@@ -19577,14 +19578,14 @@
       </c>
       <c r="X39" s="57">
         <f>MIN(X14:X34)</f>
-        <v>-0.10811107452529908</v>
+        <v>-0.24741506646971936</v>
       </c>
       <c r="Z39" t="s">
         <v>97</v>
       </c>
       <c r="AA39" s="57">
         <f>MIN(AA14:AA34)</f>
-        <v>-5.9708400833140475E-2</v>
+        <v>-0.15941431222932564</v>
       </c>
     </row>
     <row r="40" spans="7:33" x14ac:dyDescent="0.25">
@@ -19593,7 +19594,7 @@
       </c>
       <c r="O40" s="66">
         <f>P36-V36</f>
-        <v>980.5</v>
+        <v>747.00000000000091</v>
       </c>
       <c r="P40" t="str">
         <f t="shared" ref="P40:P41" si="29">IF(O40&gt;0,"Over Budget","Under Budget")</f>
@@ -19604,14 +19605,14 @@
       </c>
       <c r="X40" s="57">
         <f>MAX(X14:X34)</f>
-        <v>0.44281138119464858</v>
+        <v>0.16703703703703704</v>
       </c>
       <c r="Z40" t="s">
         <v>98</v>
       </c>
       <c r="AA40" s="57">
         <f>MAX(AA14:AA34)</f>
-        <v>0.20424403183023873</v>
+        <v>0.20436018957345972</v>
       </c>
     </row>
     <row r="41" spans="7:33" x14ac:dyDescent="0.25">
@@ -19620,7 +19621,7 @@
       </c>
       <c r="O41" s="66">
         <f>Q36-W36</f>
-        <v>-4120.5</v>
+        <v>-3313.6999999999971</v>
       </c>
       <c r="P41" t="str">
         <f t="shared" si="29"/>
@@ -19631,14 +19632,14 @@
       </c>
       <c r="X41" s="57">
         <f>MIN(Y14:Y34)</f>
-        <v>-0.43386243386243384</v>
+        <v>-0.55285961871750433</v>
       </c>
       <c r="Z41" t="s">
         <v>100</v>
       </c>
       <c r="AA41" s="57">
         <f>MIN(AB14:AB34)</f>
-        <v>-0.4514285714285714</v>
+        <v>-0.45142857142857135</v>
       </c>
     </row>
     <row r="42" spans="7:33" x14ac:dyDescent="0.25">
@@ -19648,14 +19649,14 @@
       </c>
       <c r="X42" s="57">
         <f>MAX(Y14:Y34)</f>
-        <v>0.62352941176470589</v>
+        <v>0.46612466124661245</v>
       </c>
       <c r="Z42" t="s">
         <v>101</v>
       </c>
       <c r="AA42" s="57">
         <f>MAX(AB14:AB34)</f>
-        <v>0.54189944134078216</v>
+        <v>0.53846153846153844</v>
       </c>
     </row>
     <row r="43" spans="7:33" x14ac:dyDescent="0.25">
@@ -19680,18 +19681,17 @@
       </c>
       <c r="X44" s="57">
         <f>MAX(Z14:Z34)</f>
-        <v>0.13651804670912951</v>
+        <v>0.136474609375</v>
       </c>
       <c r="Z44" t="s">
         <v>103</v>
       </c>
       <c r="AA44" s="57">
         <f>MAX(AC14:AC34)</f>
-        <v>6.6111985608275248E-2</v>
+        <v>9.6153846153846159E-2</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="Pxw+3PJEioNDA1Ga/vOsxrxc9YJQnFL5x3JlmyOfzkJ1psvTkaeWgwuaEDBMmKvXVKtqTNTlSkaY/hmIOhjFqg==" saltValue="l9d5d7nwgEtHHXOAcKQlBQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>

</xml_diff>